<commit_message>
updates for summer 22
</commit_message>
<xml_diff>
--- a/KurseMscECMX_SoSe22.xlsx
+++ b/KurseMscECMX_SoSe22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Git_projects/ECMTX_course_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEADDB5-D20A-8C47-9CCD-608CCEDFE3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBAB8D2-08E2-2A4E-9B08-8507BF0147D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Kursliste" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kursliste!$A$1:$K$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kursliste!$A$1:$K$96</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Liste!$A$1:$C$38</definedName>
     <definedName name="Anfangszeit" localSheetId="0">#REF!</definedName>
     <definedName name="Anfangszeit">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="354">
   <si>
     <t>Kurs</t>
   </si>
@@ -503,9 +503,6 @@
   </si>
   <si>
     <t>Seminar on Health Economics and Health Policy</t>
-  </si>
-  <si>
-    <t>Advanced Microeconomics</t>
   </si>
   <si>
     <t>Prof. Dr. Jörg Schimmelpfennig</t>
@@ -927,9 +924,6 @@
   </si>
   <si>
     <t>https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=vvz&amp;gguid=0xB253EECD61384EDE9DE895AE30435AD4&amp;mode=own&amp;lang=en&amp;tguid=0x80B5E42E2E744540BF79A272358D1095</t>
-  </si>
-  <si>
-    <t>https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=&amp;gguid=0x51E7ACC14F354022996527B9095AB7CB&amp;mode=&amp;tguid=0x80B5E42E2E744540BF79A272358D1095&amp;lang=en</t>
   </si>
   <si>
     <t>https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?gguid=0xE8E555FEBFD14A8092DE2B55E7F8A524&amp;from=&amp;tabID=1&amp;tguid=0x80B5E42E2E744540BF79A272358D1095&amp;objgguid=NEW&amp;lang=en</t>
@@ -1943,10 +1937,10 @@
         <v>88</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -1954,10 +1948,10 @@
         <v>91</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -1965,7 +1959,7 @@
         <v>92</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>127</v>
@@ -1976,21 +1970,21 @@
         <v>137</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -1998,43 +1992,43 @@
         <v>98</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>220</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2042,7 +2036,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>119</v>
@@ -2053,7 +2047,7 @@
         <v>122</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>120</v>
@@ -2064,7 +2058,7 @@
         <v>113</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>123</v>
@@ -2072,10 +2066,10 @@
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>139</v>
@@ -2083,24 +2077,24 @@
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2108,7 +2102,7 @@
         <v>64</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>124</v>
@@ -2119,7 +2113,7 @@
         <v>79</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>125</v>
@@ -2130,7 +2124,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>126</v>
@@ -2141,7 +2135,7 @@
         <v>138</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>128</v>
@@ -2152,7 +2146,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>133</v>
@@ -2160,10 +2154,10 @@
     </row>
     <row r="22" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>135</v>
@@ -2174,7 +2168,7 @@
         <v>77</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>136</v>
@@ -2185,7 +2179,7 @@
         <v>83</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>150</v>
@@ -2210,7 +2204,7 @@
         <v>121</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2218,21 +2212,21 @@
         <v>15</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="33" t="s">
         <v>208</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2240,10 +2234,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2251,7 +2245,7 @@
         <v>100</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>129</v>
@@ -2262,7 +2256,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>130</v>
@@ -2273,7 +2267,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>131</v>
@@ -2284,7 +2278,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>132</v>
@@ -2295,10 +2289,10 @@
         <v>30</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="33" t="s">
         <v>213</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="1" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2306,7 +2300,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>134</v>
@@ -2317,10 +2311,10 @@
         <v>49</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="1" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2339,7 +2333,7 @@
         <v>147</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>148</v>
@@ -2347,13 +2341,13 @@
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2745,13 +2739,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMD98"/>
+  <dimension ref="A1:AMD97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2794,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>103</v>
@@ -2808,10 +2802,10 @@
     </row>
     <row r="2" spans="1:11" s="18" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="31" t="str">
         <f>VLOOKUP($E2,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -2830,7 +2824,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I2" s="40">
         <v>3</v>
@@ -2844,10 +2838,10 @@
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C3" s="31" t="str">
         <f>VLOOKUP($E3,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -2866,7 +2860,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I3" s="40">
         <v>4</v>
@@ -2893,7 +2887,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>53</v>
@@ -2902,7 +2896,7 @@
         <v>42</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I4" s="41">
         <v>5</v>
@@ -2938,7 +2932,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I5" s="41">
         <v>6</v>
@@ -2952,10 +2946,10 @@
     </row>
     <row r="6" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>141</v>
@@ -2964,7 +2958,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>53</v>
@@ -2973,7 +2967,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I6" s="41">
         <v>50</v>
@@ -3000,7 +2994,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>53</v>
@@ -3009,7 +3003,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I7" s="40">
         <v>7</v>
@@ -3023,98 +3017,101 @@
     </row>
     <row r="8" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>154</v>
+        <v>90</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C8" s="38" t="str">
         <f>VLOOKUP($E8,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Theoretical and Applied Microeconomics</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="26" t="s">
+        <v>Adjunct Professorship of Health Economics</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>10</v>
+      <c r="G8" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>109</v>
+        <v>301</v>
+      </c>
+      <c r="I8" s="27">
+        <v>17</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>90</v>
+        <v>156</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="C9" s="38" t="str">
         <f>VLOOKUP($E9,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Adjunct Professorship of Health Economics</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>91</v>
+        <v>Chair of Macroeconomics</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H9" s="45" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I9" s="27">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="26" t="s">
-        <v>157</v>
+        <v>333</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="38" t="str">
-        <f>VLOOKUP($E10,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Macroeconomics</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>333</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>158</v>
+        <v>334</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>89</v>
+        <v>335</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="45" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
       <c r="I10" s="27">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>11</v>
@@ -3125,31 +3122,30 @@
     </row>
     <row r="11" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>335</v>
+        <v>161</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>335</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>339</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C11" s="38" t="str">
+        <f>VLOOKUP($E11,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Applied Microeconomics</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="8" t="s">
-        <v>336</v>
+        <v>162</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>337</v>
+        <v>89</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="45" t="s">
-        <v>338</v>
+        <v>292</v>
       </c>
       <c r="I11" s="27">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>11</v>
@@ -3160,90 +3156,90 @@
     </row>
     <row r="12" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>162</v>
+        <v>94</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="C12" s="38" t="str">
         <f>VLOOKUP($E12,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Applied Microeconomics</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="8" t="s">
-        <v>163</v>
+        <v>Chair of Public Finance and Economic Policy</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="I12" s="27">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="C13" s="38" t="str">
         <f>VLOOKUP($E13,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Public Finance and Economic Policy</v>
+        <v>Adjunct Professorship of Health Economics</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="I13" s="27">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C14" s="38" t="str">
         <f>VLOOKUP($E14,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Adjunct Professorship of Health Economics</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>Chair of Statistics/Econometrics</v>
+      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>89</v>
@@ -3252,10 +3248,10 @@
         <v>10</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I14" s="27">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>11</v>
@@ -3266,16 +3262,18 @@
     </row>
     <row r="15" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="26" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="C15" s="38" t="str">
         <f>VLOOKUP($E15,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Statistics/Econometrics</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="E15" s="12" t="s">
         <v>88</v>
       </c>
@@ -3283,73 +3281,72 @@
         <v>89</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="I15" s="27">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="38" t="str">
+        <v>166</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="26" t="str">
         <f>VLOOKUP($E16,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics/Econometrics</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="12" t="s">
+        <v>Chair of Empirical Economics</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>16</v>
+      <c r="G16" s="26" t="s">
+        <v>10</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>305</v>
-      </c>
-      <c r="I16" s="27">
-        <v>25</v>
-      </c>
-      <c r="J16" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="I16" s="37">
+        <v>26</v>
+      </c>
+      <c r="J16" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>108</v>
+      <c r="K16" s="26" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="26" t="s">
-        <v>167</v>
+        <v>338</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="26" t="str">
-        <f>VLOOKUP($E17,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Empirical Economics</v>
+        <v>338</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>341</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>92</v>
+        <v>339</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>89</v>
@@ -3357,11 +3354,11 @@
       <c r="G17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="45" t="s">
-        <v>306</v>
+      <c r="H17" s="47" t="s">
+        <v>340</v>
       </c>
       <c r="I17" s="37">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>11</v>
@@ -3372,31 +3369,32 @@
     </row>
     <row r="18" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="26" t="s">
-        <v>340</v>
+        <v>167</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>340</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>343</v>
+        <v>167</v>
+      </c>
+      <c r="C18" s="26" t="str">
+        <f>VLOOKUP($E18,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Empirical Economics</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>341</v>
+        <v>92</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="47" t="s">
-        <v>342</v>
+        <v>16</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>304</v>
       </c>
       <c r="I18" s="37">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J18" s="26" t="s">
         <v>11</v>
@@ -3407,53 +3405,53 @@
     </row>
     <row r="19" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="26" t="str">
+        <v>93</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="16" t="str">
         <f>VLOOKUP($E19,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Empirical Economics</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>306</v>
-      </c>
-      <c r="I19" s="37">
-        <v>28</v>
-      </c>
-      <c r="J19" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I19" s="27">
+        <v>29</v>
+      </c>
+      <c r="J19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="26" t="s">
-        <v>109</v>
+      <c r="K19" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="26" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C20" s="16" t="str">
         <f>VLOOKUP($E20,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Empirical Economics</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>92</v>
@@ -3462,49 +3460,49 @@
         <v>89</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="I20" s="27">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="C21" s="16" t="str">
         <f>VLOOKUP($E21,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Empirical Economics</v>
+        <v>Chair of Statistics/Econometrics</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>260</v>
+        <v>295</v>
       </c>
       <c r="I21" s="27">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>11</v>
@@ -3515,89 +3513,89 @@
     </row>
     <row r="22" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>70</v>
+        <v>152</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>152</v>
       </c>
       <c r="C22" s="16" t="str">
         <f>VLOOKUP($E22,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics/Econometrics</v>
+        <v>Chair of Empirical Economics</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="I22" s="27">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J22" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>152</v>
+        <v>99</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="C23" s="16" t="str">
         <f>VLOOKUP($E23,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Empirical Economics</v>
+        <v>Chair of Statistics/Econometrics</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>16</v>
+        <v>297</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="I23" s="27">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C24" s="16" t="str">
         <f>VLOOKUP($E24,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Statistics/Econometrics</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>88</v>
@@ -3606,37 +3604,37 @@
         <v>89</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>299</v>
+        <v>42</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="I24" s="27">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>96</v>
+        <v>255</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="16" t="str">
         <f>VLOOKUP($E25,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics/Econometrics</v>
+        <v>Chair of Economic Policy and Applied Econometrics</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>89</v>
@@ -3645,10 +3643,10 @@
         <v>42</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I25" s="27">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J25" s="12" t="s">
         <v>11</v>
@@ -3657,93 +3655,93 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="16" t="str">
+    <row r="26" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="14" t="str">
         <f>VLOOKUP($E26,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Economic Policy and Applied Econometrics</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>42</v>
+        <v>Professorship of Applied Economics</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="H26" s="45" t="s">
-        <v>310</v>
-      </c>
-      <c r="I26" s="27">
-        <v>35</v>
-      </c>
-      <c r="J26" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="I26" s="40">
+        <v>36</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="10" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
-        <v>50</v>
+        <v>342</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="14" t="str">
-        <f>VLOOKUP($E27,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Applied Economics</v>
+        <v>342</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>344</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>52</v>
+        <v>345</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H27" s="45" t="s">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c r="I27" s="40">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J27" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="19" t="s">
-        <v>344</v>
+        <v>65</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>346</v>
+        <v>66</v>
+      </c>
+      <c r="C28" s="14" t="str">
+        <f>VLOOKUP($E28,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Professorship Macroeconomics</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>347</v>
+        <v>67</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>53</v>
@@ -3752,10 +3750,10 @@
         <v>10</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>345</v>
+        <v>273</v>
       </c>
       <c r="I28" s="40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>11</v>
@@ -3765,33 +3763,33 @@
       </c>
     </row>
     <row r="29" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="19" t="s">
-        <v>65</v>
+      <c r="A29" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C29" s="14" t="str">
         <f>VLOOKUP($E29,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship Macroeconomics</v>
+        <v>Chair of Microeconomic Theory</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="H29" s="45" t="s">
-        <v>274</v>
+        <v>232</v>
       </c>
       <c r="I29" s="40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>11</v>
@@ -3801,147 +3799,145 @@
       </c>
     </row>
     <row r="30" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="10" t="s">
+      <c r="A30" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="14" t="str">
+      <c r="C30" s="31" t="str">
         <f>VLOOKUP($E30,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Microeconomic Theory</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>175</v>
       </c>
       <c r="H30" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="41">
         <v>39</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="31" t="str">
+      <c r="C31" s="14" t="str">
         <f>VLOOKUP($E31,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Microeconomic Theory</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>14</v>
+      <c r="D31" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>175</v>
       </c>
       <c r="H31" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="I31" s="41">
+      <c r="I31" s="40">
         <v>39</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="10" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C32" s="14" t="str">
         <f>VLOOKUP($E32,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Microeconomic Theory</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H32" s="45" t="s">
-        <v>235</v>
+        <v>310</v>
       </c>
       <c r="I32" s="40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J32" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="19" t="s">
-        <v>72</v>
+        <v>175</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
       <c r="C33" s="14" t="str">
         <f>VLOOKUP($E33,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Microeconomic Theory</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>14</v>
-      </c>
+        <v>Faculty of Statistics</v>
+      </c>
+      <c r="D33" s="10"/>
       <c r="E33" s="10" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="H33" s="45" t="s">
-        <v>312</v>
+        <v>242</v>
       </c>
       <c r="I33" s="40">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -3949,7 +3945,7 @@
         <v>176</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C34" s="14" t="str">
         <f>VLOOKUP($E34,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -3965,9 +3961,7 @@
       <c r="G34" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="45" t="s">
-        <v>243</v>
-      </c>
+      <c r="H34" s="45"/>
       <c r="I34" s="40">
         <v>41</v>
       </c>
@@ -3980,28 +3974,32 @@
     </row>
     <row r="35" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="19" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>178</v>
+        <v>58</v>
       </c>
       <c r="C35" s="14" t="str">
         <f>VLOOKUP($E35,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
-      </c>
-      <c r="D35" s="10"/>
+        <v>Professorship of Applied Economics</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="E35" s="10" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="I35" s="40">
         <v>42</v>
-      </c>
-      <c r="H35" s="45"/>
-      <c r="I35" s="40">
-        <v>41</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>37</v>
@@ -4012,7 +4010,7 @@
     </row>
     <row r="36" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="19" t="s">
-        <v>57</v>
+        <v>243</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>58</v>
@@ -4031,10 +4029,10 @@
         <v>53</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H36" s="45" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="I36" s="40">
         <v>42</v>
@@ -4043,22 +4041,22 @@
         <v>37</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="19" t="s">
-        <v>244</v>
+        <v>55</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" s="14" t="str">
         <f>VLOOKUP($E37,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Professorship of Applied Economics</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>52</v>
@@ -4067,13 +4065,13 @@
         <v>53</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="H37" s="45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I37" s="40">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>37</v>
@@ -4084,20 +4082,20 @@
     </row>
     <row r="38" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="19" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C38" s="14" t="str">
         <f>VLOOKUP($E38,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Applied Economics</v>
+        <v>Professorship of Finance</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>53</v>
@@ -4106,13 +4104,13 @@
         <v>16</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I38" s="40">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>108</v>
@@ -4120,17 +4118,17 @@
     </row>
     <row r="39" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="19" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C39" s="14" t="str">
         <f>VLOOKUP($E39,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Professorship of Finance</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>60</v>
@@ -4139,34 +4137,34 @@
         <v>53</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H39" s="45" t="s">
-        <v>315</v>
-      </c>
-      <c r="I39" s="40">
-        <v>44</v>
+        <v>272</v>
+      </c>
+      <c r="I39" s="42">
+        <v>45</v>
       </c>
       <c r="J39" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="19" t="s">
-        <v>70</v>
+        <v>274</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C40" s="14" t="str">
         <f>VLOOKUP($E40,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Professorship of Finance</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>60</v>
@@ -4175,71 +4173,69 @@
         <v>53</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H40" s="45" t="s">
-        <v>273</v>
-      </c>
-      <c r="I40" s="42">
-        <v>45</v>
+        <v>314</v>
+      </c>
+      <c r="I40" s="40">
+        <v>46</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>11</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="19" t="s">
-        <v>275</v>
+        <v>75</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" s="14" t="str">
         <f>VLOOKUP($E41,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Finance</v>
+        <v>Chair of Economic Policy</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H41" s="45" t="s">
-        <v>316</v>
+        <v>244</v>
       </c>
       <c r="I41" s="40">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="19" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
       <c r="C42" s="14" t="str">
         <f>VLOOKUP($E42,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Economic Policy</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>14</v>
-      </c>
+      <c r="D42" s="10"/>
       <c r="E42" s="10" t="s">
         <v>77</v>
       </c>
@@ -4247,80 +4243,82 @@
         <v>53</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="I42" s="40">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="19" t="s">
-        <v>180</v>
+        <v>54</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C43" s="14" t="str">
+        <v>110</v>
+      </c>
+      <c r="C43" s="31" t="str">
         <f>VLOOKUP($E43,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Economic Policy</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F43" s="10" t="s">
+        <v>Faculty of Statistics</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="19" t="s">
         <v>42</v>
       </c>
       <c r="H43" s="45" t="s">
-        <v>317</v>
-      </c>
-      <c r="I43" s="40">
-        <v>48</v>
-      </c>
-      <c r="J43" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+        <v>245</v>
+      </c>
+      <c r="I43" s="41">
+        <v>50</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="19" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="31" t="str">
+      <c r="C44" s="14" t="str">
         <f>VLOOKUP($E44,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
-      </c>
-      <c r="D44" s="19" t="s">
+        <v>Chair of Statistical Methods for Big Data</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F44" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G44" s="19" t="s">
         <v>42</v>
       </c>
       <c r="H44" s="45" t="s">
-        <v>246</v>
+        <v>316</v>
       </c>
       <c r="I44" s="41">
         <v>50</v>
@@ -4328,76 +4326,74 @@
       <c r="J44" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K44" s="19" t="s">
-        <v>109</v>
+      <c r="K44" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="19" t="s">
-        <v>114</v>
+        <v>266</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="14" t="str">
-        <f>VLOOKUP($E45,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistical Methods for Big Data</v>
+        <v>266</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>113</v>
+        <v>268</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>318</v>
+        <v>267</v>
       </c>
       <c r="I45" s="41">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="19" t="s">
-        <v>267</v>
+        <v>12</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>141</v>
+        <v>110</v>
+      </c>
+      <c r="C46" s="14" t="str">
+        <f>VLOOKUP($E46,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>269</v>
+        <v>140</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="45" t="s">
-        <v>268</v>
-      </c>
-      <c r="I46" s="41">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="H46" s="45"/>
+      <c r="I46" s="40">
+        <v>50</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K46" s="10" t="s">
         <v>109</v>
@@ -4405,28 +4401,30 @@
     </row>
     <row r="47" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="19" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C47" s="14" t="str">
         <f>VLOOKUP($E47,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
+        <v>Chair of Mathematical Statistics with Applications in Biometrics</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H47" s="45"/>
+        <v>16</v>
+      </c>
+      <c r="H47" s="45" t="s">
+        <v>317</v>
+      </c>
       <c r="I47" s="40">
         <v>50</v>
       </c>
@@ -4434,34 +4432,34 @@
         <v>37</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C48" s="14" t="str">
         <f>VLOOKUP($E48,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Mathematical Statistics with Applications in Biometrics</v>
+        <v>Chair of Business and Social Statistics</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H48" s="45" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
       <c r="I48" s="40">
         <v>50</v>
@@ -4470,25 +4468,25 @@
         <v>37</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
-        <v>276</v>
+        <v>180</v>
       </c>
       <c r="B49" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C49" s="14" t="str">
         <f>VLOOKUP($E49,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Business and Social Statistics</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>53</v>
@@ -4496,9 +4494,7 @@
       <c r="G49" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H49" s="45" t="s">
-        <v>277</v>
-      </c>
+      <c r="H49" s="45"/>
       <c r="I49" s="40">
         <v>50</v>
       </c>
@@ -4511,9 +4507,9 @@
     </row>
     <row r="50" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="B50" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C50" s="14" t="str">
@@ -4521,7 +4517,7 @@
         <v>Faculty of Statistics</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>140</v>
@@ -4534,7 +4530,7 @@
       </c>
       <c r="H50" s="45"/>
       <c r="I50" s="40">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J50" s="19" t="s">
         <v>37</v>
@@ -4545,7 +4541,7 @@
     </row>
     <row r="51" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="19" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>110</v>
@@ -4566,9 +4562,11 @@
       <c r="G51" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="45"/>
+      <c r="H51" s="45" t="s">
+        <v>235</v>
+      </c>
       <c r="I51" s="40">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J51" s="19" t="s">
         <v>37</v>
@@ -4579,7 +4577,7 @@
     </row>
     <row r="52" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>110</v>
@@ -4615,7 +4613,7 @@
     </row>
     <row r="53" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="19" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>110</v>
@@ -4651,17 +4649,17 @@
     </row>
     <row r="54" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="19" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="14" t="str">
+      <c r="C54" s="29" t="str">
         <f>VLOOKUP($E54,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>140</v>
@@ -4687,17 +4685,17 @@
     </row>
     <row r="55" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="19" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="29" t="str">
+      <c r="C55" s="14" t="str">
         <f>VLOOKUP($E55,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>140</v>
@@ -4723,7 +4721,7 @@
     </row>
     <row r="56" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="19" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>110</v>
@@ -4759,7 +4757,7 @@
     </row>
     <row r="57" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="19" t="s">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>110</v>
@@ -4769,7 +4767,7 @@
         <v>Faculty of Statistics</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>14</v>
+        <v>319</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>140</v>
@@ -4781,7 +4779,7 @@
         <v>42</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>241</v>
+        <v>318</v>
       </c>
       <c r="I57" s="40">
         <v>50</v>
@@ -4795,7 +4793,7 @@
     </row>
     <row r="58" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="19" t="s">
-        <v>182</v>
+        <v>85</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>110</v>
@@ -4805,7 +4803,7 @@
         <v>Faculty of Statistics</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>321</v>
+        <v>14</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>140</v>
@@ -4817,7 +4815,7 @@
         <v>42</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>320</v>
+        <v>246</v>
       </c>
       <c r="I58" s="40">
         <v>50</v>
@@ -4831,19 +4829,19 @@
     </row>
     <row r="59" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="19" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C59" s="14" t="str">
         <f>VLOOKUP($E59,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="44" t="s">
         <v>140</v>
       </c>
       <c r="F59" s="10" t="s">
@@ -4852,13 +4850,11 @@
       <c r="G59" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H59" s="45" t="s">
-        <v>247</v>
-      </c>
+      <c r="H59" s="45"/>
       <c r="I59" s="40">
-        <v>50</v>
-      </c>
-      <c r="J59" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J59" s="10" t="s">
         <v>37</v>
       </c>
       <c r="K59" s="10" t="s">
@@ -4867,20 +4863,20 @@
     </row>
     <row r="60" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="19" t="s">
-        <v>183</v>
+        <v>265</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>96</v>
       </c>
       <c r="C60" s="14" t="str">
         <f>VLOOKUP($E60,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
+        <v>Chair of Business and Social Statistics</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="44" t="s">
-        <v>140</v>
+      <c r="E60" s="10" t="s">
+        <v>138</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>53</v>
@@ -4888,7 +4884,9 @@
       <c r="G60" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H60" s="45"/>
+      <c r="H60" s="45" t="s">
+        <v>264</v>
+      </c>
       <c r="I60" s="40">
         <v>52</v>
       </c>
@@ -4901,35 +4899,35 @@
     </row>
     <row r="61" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="19" t="s">
-        <v>266</v>
+        <v>74</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C61" s="14" t="str">
         <f>VLOOKUP($E61,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Business and Social Statistics</v>
+        <v>Chair of Artificial Intelligence</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H61" s="45" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="I61" s="40">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K61" s="10" t="s">
         <v>109</v>
@@ -4937,91 +4935,90 @@
     </row>
     <row r="62" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="14" t="str">
+        <v>86</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="31" t="str">
         <f>VLOOKUP($E62,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Artificial Intelligence</v>
       </c>
-      <c r="D62" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="F62" s="10" t="s">
+      <c r="D62" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F62" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="19"/>
+      <c r="H62" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="I62" s="41">
+        <v>54</v>
+      </c>
+      <c r="J62" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="15" t="str">
+        <f>VLOOKUP($E63,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Environmental Economics,
+ esp. Economics of Renewable Energy</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H62" s="45" t="s">
+      <c r="H63" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="I62" s="40">
-        <v>53</v>
-      </c>
-      <c r="J62" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K62" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="31" t="str">
-        <f>VLOOKUP($E63,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Artificial Intelligence</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G63" s="19"/>
-      <c r="H63" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="I63" s="41">
-        <v>54</v>
-      </c>
-      <c r="J63" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="K63" s="19" t="s">
+      <c r="I63" s="39">
+        <v>55</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K63" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="21" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="15" t="str">
-        <f>VLOOKUP($E64,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Environmental Economics,
- esp. Economics of Renewable Energy</v>
+        <v>346</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>111</v>
+        <v>347</v>
       </c>
       <c r="F64" s="11" t="s">
         <v>9</v>
@@ -5030,10 +5027,10 @@
         <v>10</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>279</v>
+        <v>348</v>
       </c>
       <c r="I64" s="39">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J64" s="11" t="s">
         <v>11</v>
@@ -5044,108 +5041,109 @@
     </row>
     <row r="65" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="21" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>121</v>
+        <v>352</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F65" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="47" t="s">
         <v>350</v>
       </c>
       <c r="I65" s="39">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J65" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="21" t="s">
-        <v>351</v>
+        <v>20</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>354</v>
+        <v>20</v>
+      </c>
+      <c r="C66" s="15" t="str">
+        <f>VLOOKUP($E66,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Microeconomics</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>353</v>
+        <v>21</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H66" s="47" t="s">
-        <v>352</v>
-      </c>
-      <c r="I66" s="39">
-        <v>57</v>
-      </c>
-      <c r="J66" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K66" s="11" t="s">
-        <v>108</v>
+        <v>22</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="I66" s="24">
+        <v>58</v>
+      </c>
+      <c r="J66" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K66" s="25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="21" t="s">
-        <v>20</v>
+        <v>184</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>20</v>
+        <v>184</v>
       </c>
       <c r="C67" s="15" t="str">
         <f>VLOOKUP($E67,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Microeconomics</v>
+        <v>Chair of International Economics</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G67" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H67" s="45" t="s">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="I67" s="24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -5157,229 +5155,229 @@
       </c>
       <c r="C68" s="15" t="str">
         <f>VLOOKUP($E68,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of International Economics</v>
+        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="F68" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G68" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H68" s="45" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
       <c r="I68" s="24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J68" s="23" t="s">
         <v>11</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C69" s="15" t="str">
+        <v>143</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="35" t="str">
         <f>VLOOKUP($E69,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="E69" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="22" t="s">
-        <v>10</v>
+      <c r="G69" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="H69" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="I69" s="24">
-        <v>60</v>
-      </c>
-      <c r="J69" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="I69" s="36">
+        <v>61</v>
+      </c>
+      <c r="J69" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K69" s="25" t="s">
-        <v>109</v>
+      <c r="K69" s="21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B70" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C70" s="35" t="str">
+        <v>40</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="15" t="str">
         <f>VLOOKUP($E70,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
-      </c>
-      <c r="D70" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F70" s="21" t="s">
+        <v>Chair of Microeconomics</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G70" s="21" t="s">
-        <v>16</v>
+      <c r="G70" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="H70" s="45" t="s">
-        <v>323</v>
-      </c>
-      <c r="I70" s="36">
-        <v>61</v>
-      </c>
-      <c r="J70" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="K70" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="I70" s="24">
+        <v>62</v>
+      </c>
+      <c r="J70" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K70" s="25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C71" s="15" t="str">
+        <v>149</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C71" s="35" t="str">
         <f>VLOOKUP($E71,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Microeconomics</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71" s="11" t="s">
+        <v>Chair of Labour and Health Economics</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F71" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G71" s="22" t="s">
-        <v>42</v>
+      <c r="G71" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>324</v>
-      </c>
-      <c r="I71" s="24">
-        <v>62</v>
-      </c>
-      <c r="J71" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K71" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="I71" s="36">
+        <v>63</v>
+      </c>
+      <c r="J71" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K71" s="21" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="21" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="C72" s="35" t="str">
         <f>VLOOKUP($E72,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
       </c>
       <c r="D72" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="21" t="s">
-        <v>147</v>
+      <c r="E72" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="F72" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="I72" s="36">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J72" s="21" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K72" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="21" t="s">
-        <v>187</v>
+        <v>256</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C73" s="35" t="str">
+        <v>256</v>
+      </c>
+      <c r="C73" s="15" t="str">
         <f>VLOOKUP($E73,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
-      </c>
-      <c r="D73" s="21" t="s">
+        <v>Chair of Public Economics</v>
+      </c>
+      <c r="D73" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F73" s="21" t="s">
+      <c r="E73" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F73" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G73" s="21" t="s">
-        <v>10</v>
+      <c r="G73" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="H73" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="I73" s="36">
-        <v>64</v>
-      </c>
-      <c r="J73" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K73" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="I73" s="24">
+        <v>65</v>
+      </c>
+      <c r="J73" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K73" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="B74" s="21" t="s">
-        <v>257</v>
+        <v>47</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C74" s="15" t="str">
         <f>VLOOKUP($E74,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Public Economics</v>
+        <v>Chair of Finance</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F74" s="11" t="s">
         <v>9</v>
@@ -5391,10 +5389,10 @@
         <v>249</v>
       </c>
       <c r="I74" s="24">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J74" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K74" s="25" t="s">
         <v>109</v>
@@ -5402,129 +5400,129 @@
     </row>
     <row r="75" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="21" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C75" s="15" t="str">
         <f>VLOOKUP($E75,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Finance</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F75" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G75" s="22" t="s">
+      <c r="G75" s="11" t="s">
         <v>16</v>
       </c>
       <c r="H75" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="I75" s="24">
-        <v>67</v>
-      </c>
-      <c r="J75" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="I75" s="39">
+        <v>69</v>
+      </c>
+      <c r="J75" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K75" s="25" t="s">
-        <v>109</v>
+      <c r="K75" s="11" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>106</v>
+        <v>187</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="C76" s="15" t="str">
         <f>VLOOKUP($E76,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of Labour and Health Economics</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>326</v>
+        <v>282</v>
       </c>
       <c r="I76" s="39">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J76" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K76" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B77" s="21" t="s">
-        <v>188</v>
+        <v>24</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C77" s="15" t="str">
         <f>VLOOKUP($E77,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Chair of Environmental Economics,
+ esp. Economics of Renewable Energy</v>
       </c>
       <c r="D77" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E77" s="21" t="s">
-        <v>147</v>
+      <c r="E77" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G77" s="11" t="s">
-        <v>10</v>
+      <c r="G77" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="H77" s="45" t="s">
-        <v>283</v>
-      </c>
-      <c r="I77" s="39">
-        <v>70</v>
-      </c>
-      <c r="J77" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="I77" s="24">
+        <v>71</v>
+      </c>
+      <c r="J77" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K77" s="11" t="s">
-        <v>109</v>
+      <c r="K77" s="25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C78" s="15" t="str">
         <f>VLOOKUP($E78,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Environmental Economics,
- esp. Economics of Renewable Energy</v>
+        <v>Chair of Statistics</v>
       </c>
       <c r="D78" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>9</v>
@@ -5533,13 +5531,13 @@
         <v>16</v>
       </c>
       <c r="H78" s="45" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I78" s="24">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K78" s="25" t="s">
         <v>108</v>
@@ -5547,59 +5545,59 @@
     </row>
     <row r="79" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="21" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>26</v>
+        <v>188</v>
       </c>
       <c r="C79" s="15" t="str">
         <f>VLOOKUP($E79,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
+        <v>Chair of Finance</v>
       </c>
       <c r="D79" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G79" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H79" s="45" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="I79" s="24">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="21" t="s">
-        <v>189</v>
+        <v>28</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>189</v>
+        <v>28</v>
       </c>
       <c r="C80" s="15" t="str">
         <f>VLOOKUP($E80,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Finance</v>
+        <v>Chair of Statistics</v>
       </c>
       <c r="D80" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>190</v>
+        <v>27</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>191</v>
+        <v>9</v>
       </c>
       <c r="G80" s="22" t="s">
         <v>10</v>
@@ -5608,10 +5606,10 @@
         <v>284</v>
       </c>
       <c r="I80" s="24">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K80" s="25" t="s">
         <v>109</v>
@@ -5619,20 +5617,20 @@
     </row>
     <row r="81" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C81" s="15" t="str">
         <f>VLOOKUP($E81,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
+        <v>Chair for Energy Trading and Finance</v>
       </c>
       <c r="D81" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F81" s="11" t="s">
         <v>9</v>
@@ -5644,10 +5642,10 @@
         <v>285</v>
       </c>
       <c r="I81" s="24">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>109</v>
@@ -5655,10 +5653,10 @@
     </row>
     <row r="82" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C82" s="15" t="str">
         <f>VLOOKUP($E82,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -5680,7 +5678,7 @@
         <v>286</v>
       </c>
       <c r="I82" s="24">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J82" s="23" t="s">
         <v>11</v>
@@ -5691,20 +5689,20 @@
     </row>
     <row r="83" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C83" s="15" t="str">
         <f>VLOOKUP($E83,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair for Energy Trading and Finance</v>
+        <v>Chair of Health Economics</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F83" s="11" t="s">
         <v>9</v>
@@ -5716,7 +5714,7 @@
         <v>287</v>
       </c>
       <c r="I83" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J83" s="23" t="s">
         <v>11</v>
@@ -5727,56 +5725,57 @@
     </row>
     <row r="84" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>32</v>
+        <v>191</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>191</v>
       </c>
       <c r="C84" s="15" t="str">
         <f>VLOOKUP($E84,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Health Economics</v>
+        <v>Chair of Labour and Health Economics</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="F84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H84" s="45" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
       <c r="I84" s="24">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J84" s="23" t="s">
         <v>11</v>
       </c>
       <c r="K84" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="B85" s="21" t="s">
-        <v>192</v>
+        <v>36</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="C85" s="15" t="str">
         <f>VLOOKUP($E85,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Chair of Environmental Economics,
+ esp. Economics of Renewable Energy</v>
       </c>
       <c r="D85" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="F85" s="11" t="s">
         <v>9</v>
@@ -5785,47 +5784,46 @@
         <v>16</v>
       </c>
       <c r="H85" s="45" t="s">
-        <v>329</v>
+        <v>247</v>
       </c>
       <c r="I85" s="24">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J85" s="23" t="s">
         <v>11</v>
       </c>
       <c r="K85" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="21" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="C86" s="15" t="str">
         <f>VLOOKUP($E86,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Environmental Economics,
- esp. Economics of Renewable Energy</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="F86" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G86" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H86" s="45" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="I86" s="24">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J86" s="23" t="s">
         <v>11</v>
@@ -5836,20 +5834,20 @@
     </row>
     <row r="87" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="21" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="C87" s="15" t="str">
         <f>VLOOKUP($E87,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of International Economics</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>9</v>
@@ -5861,10 +5859,10 @@
         <v>251</v>
       </c>
       <c r="I87" s="24">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>109</v>
@@ -5872,79 +5870,79 @@
     </row>
     <row r="88" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C88" s="15" t="str">
         <f>VLOOKUP($E88,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of International Economics</v>
+        <v>Chair for Energy Trading and Finance</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G88" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H88" s="45" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
       <c r="I88" s="24">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J88" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K88" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="21" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C89" s="15" t="str">
         <f>VLOOKUP($E89,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair for Energy Trading and Finance</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F89" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="H89" s="45" t="s">
-        <v>330</v>
+        <v>252</v>
       </c>
       <c r="I89" s="24">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J89" s="23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K89" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="21" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>13</v>
@@ -5963,7 +5961,7 @@
         <v>9</v>
       </c>
       <c r="G90" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H90" s="45" t="s">
         <v>253</v>
@@ -5980,7 +5978,7 @@
     </row>
     <row r="91" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="21" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>13</v>
@@ -5999,10 +5997,10 @@
         <v>9</v>
       </c>
       <c r="G91" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H91" s="45" t="s">
-        <v>254</v>
+        <v>353</v>
       </c>
       <c r="I91" s="24">
         <v>86</v>
@@ -6011,12 +6009,12 @@
         <v>37</v>
       </c>
       <c r="K91" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="21" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>13</v>
@@ -6035,10 +6033,10 @@
         <v>9</v>
       </c>
       <c r="G92" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H92" s="45" t="s">
-        <v>355</v>
+        <v>254</v>
       </c>
       <c r="I92" s="24">
         <v>86</v>
@@ -6047,112 +6045,112 @@
         <v>37</v>
       </c>
       <c r="K92" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="21" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C93" s="15" t="str">
         <f>VLOOKUP($E93,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of Health Economics</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F93" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G93" s="22" t="s">
-        <v>169</v>
+        <v>16</v>
       </c>
       <c r="H93" s="45" t="s">
-        <v>255</v>
+        <v>329</v>
       </c>
       <c r="I93" s="24">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J93" s="23" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K93" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="21" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>18</v>
+        <v>192</v>
       </c>
       <c r="C94" s="15" t="str">
         <f>VLOOKUP($E94,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Health Economics</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F94" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G94" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H94" s="45" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="I94" s="24">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J94" s="23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K94" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>193</v>
+        <v>43</v>
       </c>
       <c r="C95" s="15" t="str">
         <f>VLOOKUP($E95,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of Statistics</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F95" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G95" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H95" s="45" t="s">
-        <v>292</v>
+        <v>231</v>
       </c>
       <c r="I95" s="24">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J95" s="23" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K95" s="25" t="s">
         <v>109</v>
@@ -6160,17 +6158,17 @@
     </row>
     <row r="96" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C96" s="15" t="str">
         <f>VLOOKUP($E96,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Statistics</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>27</v>
@@ -6182,179 +6180,142 @@
         <v>16</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>232</v>
+        <v>330</v>
       </c>
       <c r="I96" s="24">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J96" s="23" t="s">
         <v>23</v>
       </c>
       <c r="K96" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="21" t="s">
-        <v>46</v>
+        <v>288</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>46</v>
+        <v>289</v>
       </c>
       <c r="C97" s="15" t="str">
         <f>VLOOKUP($E97,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F97" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G97" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H97" s="45" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="I97" s="24">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="J97" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K97" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="C98" s="15" t="str">
-        <f>VLOOKUP($E98,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E98" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F98" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="45" t="s">
-        <v>291</v>
-      </c>
-      <c r="I98" s="24">
-        <v>5</v>
-      </c>
-      <c r="J98" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K98" s="25" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="U55" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="U54" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"SONNTAG,MONTAG,DIENSTAG,MITTWOCH,DONNERSTAG,FREITAG,SAMSTAG"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="H8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="H20" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="H23" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="H27" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="H29" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="H30" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="H32" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="H33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="H34" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="H38" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="H39" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="H40" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="H41" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="H78" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="H91" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="H96" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="H2" r:id="rId19" xr:uid="{2B7F445A-4010-5D45-8B72-1E7FF5B85AC2}"/>
-    <hyperlink ref="H36" r:id="rId20" xr:uid="{60BFBEE5-076F-A64C-A225-ADEE1C4BD7CB}"/>
-    <hyperlink ref="H43" r:id="rId21" xr:uid="{23808E95-1E7A-0746-B8FD-00EDF2C86A74}"/>
-    <hyperlink ref="H62" r:id="rId22" xr:uid="{C2A1EBF8-E857-D545-B0EF-49D7097B7749}"/>
-    <hyperlink ref="H64" r:id="rId23" xr:uid="{7E63E588-49BB-D143-B9B4-E7580E586BAA}"/>
-    <hyperlink ref="H67" r:id="rId24" xr:uid="{F9FB12F0-5F1E-4143-8431-A414F19C6FF0}"/>
-    <hyperlink ref="H71" r:id="rId25" xr:uid="{9ADB501C-CF4E-DE42-829E-1B0FF8166250}"/>
-    <hyperlink ref="H80" r:id="rId26" xr:uid="{732233EA-CE2C-9B48-A34F-19AD7FDC6D2C}"/>
-    <hyperlink ref="H81" r:id="rId27" xr:uid="{4DCAD565-04BA-AD49-AD0C-4AFEB7188DCC}"/>
-    <hyperlink ref="H82" r:id="rId28" xr:uid="{F5282177-DF5F-F44C-963E-976E7C656D83}"/>
-    <hyperlink ref="H84" r:id="rId29" xr:uid="{71243A51-6FC6-E34C-90BE-9947021EA4E1}"/>
-    <hyperlink ref="H12" r:id="rId30" xr:uid="{DF1DAC8E-3F75-5846-952C-CFDFFAADB7CF}"/>
-    <hyperlink ref="H10" r:id="rId31" xr:uid="{8FB1C5CC-891B-4E45-819E-AEE1319C1CC3}"/>
-    <hyperlink ref="H14" r:id="rId32" xr:uid="{9BAEA748-035C-C844-AFBA-2E88BB1B1519}"/>
-    <hyperlink ref="H22" r:id="rId33" xr:uid="{D1D37A9C-AF90-874B-8C0B-1BA78A362FAD}"/>
-    <hyperlink ref="H4" r:id="rId34" xr:uid="{B7DEA081-AAE4-4CD0-B204-0F4244EE4D3E}"/>
-    <hyperlink ref="H5" r:id="rId35" xr:uid="{9D9B46D4-9C82-4629-81A7-EE9E91C484F1}"/>
-    <hyperlink ref="H6" r:id="rId36" xr:uid="{B5652EAC-704A-4C40-9E77-FC17CCB4C03E}"/>
-    <hyperlink ref="H7" r:id="rId37" xr:uid="{DBCA6D8E-8DA8-41DA-BC5F-E031F2C34A60}"/>
-    <hyperlink ref="H16" r:id="rId38" xr:uid="{85EBA711-3AA9-4149-8727-C59B76A32B24}"/>
-    <hyperlink ref="H17" r:id="rId39" xr:uid="{A2845418-ABCC-44FB-AD1A-91A875FC203A}"/>
-    <hyperlink ref="H19" r:id="rId40" xr:uid="{0FAD0401-1F5F-45D1-BE93-D78F79DF81F8}"/>
-    <hyperlink ref="H21" r:id="rId41" xr:uid="{EAB0A335-B193-43F5-B966-E138AD8E32FF}"/>
-    <hyperlink ref="H24" r:id="rId42" xr:uid="{3ABF5F34-0A3B-40A2-A414-5A1CC5F70788}"/>
-    <hyperlink ref="H25" r:id="rId43" xr:uid="{F3180EAA-200E-4AC7-A0C2-68DA341AE008}"/>
-    <hyperlink ref="H26" r:id="rId44" xr:uid="{9EEC934C-FC80-420E-B966-1EF8E82DD430}"/>
-    <hyperlink ref="H31" r:id="rId45" location="basicdata" xr:uid="{8C0E0B15-F2D7-4152-8A3A-C4B63DC2342A}"/>
-    <hyperlink ref="H37" r:id="rId46" xr:uid="{4DD54FB2-9139-48B1-BBCF-5D5471DAECD0}"/>
-    <hyperlink ref="H44" r:id="rId47" xr:uid="{E0310F6A-80BB-4666-B128-ABFA174004B5}"/>
-    <hyperlink ref="H45" r:id="rId48" xr:uid="{A49BCD15-895A-47E3-B38F-119C48F96EC2}"/>
-    <hyperlink ref="H48" r:id="rId49" xr:uid="{912D2986-EA6B-4EF8-8161-EB8B9777A1EA}"/>
-    <hyperlink ref="H58" r:id="rId50" xr:uid="{E4EC41F5-9B9D-4A2E-9C8D-085442A52492}"/>
-    <hyperlink ref="H59" r:id="rId51" xr:uid="{16CE3935-D21A-4C5B-82EA-1CDF0C5792B4}"/>
-    <hyperlink ref="H61" r:id="rId52" xr:uid="{95987F1E-714E-475F-9F37-BFF46E5FF853}"/>
-    <hyperlink ref="H63" r:id="rId53" xr:uid="{5573F406-C721-42E7-B33B-F5125403275C}"/>
-    <hyperlink ref="H68" r:id="rId54" xr:uid="{B09486E6-3BCF-4C35-89F1-0F55C6E5C422}"/>
-    <hyperlink ref="H70" r:id="rId55" xr:uid="{D7159F27-BE69-4A6A-88E6-12AA0DFC22B1}"/>
-    <hyperlink ref="H72" r:id="rId56" xr:uid="{32F7EAFF-4E97-4C42-B31A-A0EEEAB574D8}"/>
-    <hyperlink ref="H73" r:id="rId57" xr:uid="{BBE37BEB-91BB-454E-8C75-B096251E564C}"/>
-    <hyperlink ref="H74" r:id="rId58" xr:uid="{4246FEB6-B0C6-4315-92FF-E09E8578C666}"/>
-    <hyperlink ref="H75" r:id="rId59" xr:uid="{C3486942-4849-4ADF-9729-57579A743CBE}"/>
-    <hyperlink ref="H76" r:id="rId60" xr:uid="{74C74B68-0088-4D8D-B81A-5280BA2E3496}"/>
-    <hyperlink ref="H77" r:id="rId61" xr:uid="{3A8D2EB7-A012-4A83-86C0-51123C32DF6D}"/>
-    <hyperlink ref="H79" r:id="rId62" xr:uid="{AC284DEA-756B-4D18-AE9D-12965059EDBE}"/>
-    <hyperlink ref="H85" r:id="rId63" xr:uid="{DCB82540-1BA3-48F9-96A2-791F42A64434}"/>
-    <hyperlink ref="H86" r:id="rId64" xr:uid="{B9381049-251F-42B9-84B0-1EA59178B672}"/>
-    <hyperlink ref="H87" r:id="rId65" xr:uid="{540E3A03-74BD-4CEB-8971-9A006BEFCDF0}"/>
-    <hyperlink ref="H88" r:id="rId66" xr:uid="{72F8223A-C2F2-4F21-BABB-B8498B257A0D}"/>
-    <hyperlink ref="H89" r:id="rId67" xr:uid="{0C61D723-5ABB-4262-A872-39A6CDB6256D}"/>
-    <hyperlink ref="H90" r:id="rId68" xr:uid="{27DD1FF5-3256-41C6-B415-3EBB0EC0F4F5}"/>
-    <hyperlink ref="H94" r:id="rId69" xr:uid="{3425BE03-5207-4C7D-8D5C-A6503DADDED2}"/>
-    <hyperlink ref="H95" r:id="rId70" xr:uid="{485CFA53-D353-40F2-9341-01B79A98853E}"/>
-    <hyperlink ref="H97" r:id="rId71" xr:uid="{832E610A-F9CA-4C75-A91C-B42B0F67D4F3}"/>
-    <hyperlink ref="H98" r:id="rId72" xr:uid="{01FE6B48-CA09-4F40-B62C-9B0890D99399}"/>
-    <hyperlink ref="H3" r:id="rId73" display="https://www.lsf.tu-dortmund.de/qisserver/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=251158&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung" xr:uid="{59C03C8D-D4C1-4F3E-BE32-BECB7C56DE46}"/>
-    <hyperlink ref="H11" r:id="rId74" xr:uid="{C948447E-25EE-46B0-87D4-69726901A563}"/>
-    <hyperlink ref="H18" r:id="rId75" display="https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=vvz&amp;gguid=0xBE097E28332544129F201456DD40F8FD&amp;mode=own&amp;tguid=0x6BD942F2335C413E99E5D61BE54377E5&amp;lang=de" xr:uid="{3F957779-98BC-47BD-A023-69CBC43C874C}"/>
-    <hyperlink ref="H28" r:id="rId76" xr:uid="{58DD5441-0DE8-410C-956D-B7B8E9C3382C}"/>
-    <hyperlink ref="H65" r:id="rId77" xr:uid="{5D7A4DAF-540A-4A6F-9864-C56D22020CE4}"/>
-    <hyperlink ref="H66" r:id="rId78" xr:uid="{E793A7A2-4E6A-4865-9FD7-3E09C15CB431}"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H19" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H22" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H26" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="H28" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="H29" r:id="rId7" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="H31" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="H32" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="H33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="H37" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="H38" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="H39" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="H40" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="H77" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="H90" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="H95" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="H2" r:id="rId18" xr:uid="{2B7F445A-4010-5D45-8B72-1E7FF5B85AC2}"/>
+    <hyperlink ref="H35" r:id="rId19" xr:uid="{60BFBEE5-076F-A64C-A225-ADEE1C4BD7CB}"/>
+    <hyperlink ref="H42" r:id="rId20" xr:uid="{23808E95-1E7A-0746-B8FD-00EDF2C86A74}"/>
+    <hyperlink ref="H61" r:id="rId21" xr:uid="{C2A1EBF8-E857-D545-B0EF-49D7097B7749}"/>
+    <hyperlink ref="H63" r:id="rId22" xr:uid="{7E63E588-49BB-D143-B9B4-E7580E586BAA}"/>
+    <hyperlink ref="H66" r:id="rId23" xr:uid="{F9FB12F0-5F1E-4143-8431-A414F19C6FF0}"/>
+    <hyperlink ref="H70" r:id="rId24" xr:uid="{9ADB501C-CF4E-DE42-829E-1B0FF8166250}"/>
+    <hyperlink ref="H79" r:id="rId25" xr:uid="{732233EA-CE2C-9B48-A34F-19AD7FDC6D2C}"/>
+    <hyperlink ref="H80" r:id="rId26" xr:uid="{4DCAD565-04BA-AD49-AD0C-4AFEB7188DCC}"/>
+    <hyperlink ref="H81" r:id="rId27" xr:uid="{F5282177-DF5F-F44C-963E-976E7C656D83}"/>
+    <hyperlink ref="H83" r:id="rId28" xr:uid="{71243A51-6FC6-E34C-90BE-9947021EA4E1}"/>
+    <hyperlink ref="H11" r:id="rId29" xr:uid="{DF1DAC8E-3F75-5846-952C-CFDFFAADB7CF}"/>
+    <hyperlink ref="H9" r:id="rId30" xr:uid="{8FB1C5CC-891B-4E45-819E-AEE1319C1CC3}"/>
+    <hyperlink ref="H13" r:id="rId31" xr:uid="{9BAEA748-035C-C844-AFBA-2E88BB1B1519}"/>
+    <hyperlink ref="H21" r:id="rId32" xr:uid="{D1D37A9C-AF90-874B-8C0B-1BA78A362FAD}"/>
+    <hyperlink ref="H4" r:id="rId33" xr:uid="{B7DEA081-AAE4-4CD0-B204-0F4244EE4D3E}"/>
+    <hyperlink ref="H5" r:id="rId34" xr:uid="{9D9B46D4-9C82-4629-81A7-EE9E91C484F1}"/>
+    <hyperlink ref="H6" r:id="rId35" xr:uid="{B5652EAC-704A-4C40-9E77-FC17CCB4C03E}"/>
+    <hyperlink ref="H7" r:id="rId36" xr:uid="{DBCA6D8E-8DA8-41DA-BC5F-E031F2C34A60}"/>
+    <hyperlink ref="H15" r:id="rId37" xr:uid="{85EBA711-3AA9-4149-8727-C59B76A32B24}"/>
+    <hyperlink ref="H16" r:id="rId38" xr:uid="{A2845418-ABCC-44FB-AD1A-91A875FC203A}"/>
+    <hyperlink ref="H18" r:id="rId39" xr:uid="{0FAD0401-1F5F-45D1-BE93-D78F79DF81F8}"/>
+    <hyperlink ref="H20" r:id="rId40" xr:uid="{EAB0A335-B193-43F5-B966-E138AD8E32FF}"/>
+    <hyperlink ref="H23" r:id="rId41" xr:uid="{3ABF5F34-0A3B-40A2-A414-5A1CC5F70788}"/>
+    <hyperlink ref="H24" r:id="rId42" xr:uid="{F3180EAA-200E-4AC7-A0C2-68DA341AE008}"/>
+    <hyperlink ref="H25" r:id="rId43" xr:uid="{9EEC934C-FC80-420E-B966-1EF8E82DD430}"/>
+    <hyperlink ref="H30" r:id="rId44" location="basicdata" xr:uid="{8C0E0B15-F2D7-4152-8A3A-C4B63DC2342A}"/>
+    <hyperlink ref="H36" r:id="rId45" xr:uid="{4DD54FB2-9139-48B1-BBCF-5D5471DAECD0}"/>
+    <hyperlink ref="H43" r:id="rId46" xr:uid="{E0310F6A-80BB-4666-B128-ABFA174004B5}"/>
+    <hyperlink ref="H44" r:id="rId47" xr:uid="{A49BCD15-895A-47E3-B38F-119C48F96EC2}"/>
+    <hyperlink ref="H47" r:id="rId48" xr:uid="{912D2986-EA6B-4EF8-8161-EB8B9777A1EA}"/>
+    <hyperlink ref="H57" r:id="rId49" xr:uid="{E4EC41F5-9B9D-4A2E-9C8D-085442A52492}"/>
+    <hyperlink ref="H58" r:id="rId50" xr:uid="{16CE3935-D21A-4C5B-82EA-1CDF0C5792B4}"/>
+    <hyperlink ref="H60" r:id="rId51" xr:uid="{95987F1E-714E-475F-9F37-BFF46E5FF853}"/>
+    <hyperlink ref="H62" r:id="rId52" xr:uid="{5573F406-C721-42E7-B33B-F5125403275C}"/>
+    <hyperlink ref="H67" r:id="rId53" xr:uid="{B09486E6-3BCF-4C35-89F1-0F55C6E5C422}"/>
+    <hyperlink ref="H69" r:id="rId54" xr:uid="{D7159F27-BE69-4A6A-88E6-12AA0DFC22B1}"/>
+    <hyperlink ref="H71" r:id="rId55" xr:uid="{32F7EAFF-4E97-4C42-B31A-A0EEEAB574D8}"/>
+    <hyperlink ref="H72" r:id="rId56" xr:uid="{BBE37BEB-91BB-454E-8C75-B096251E564C}"/>
+    <hyperlink ref="H73" r:id="rId57" xr:uid="{4246FEB6-B0C6-4315-92FF-E09E8578C666}"/>
+    <hyperlink ref="H74" r:id="rId58" xr:uid="{C3486942-4849-4ADF-9729-57579A743CBE}"/>
+    <hyperlink ref="H75" r:id="rId59" xr:uid="{74C74B68-0088-4D8D-B81A-5280BA2E3496}"/>
+    <hyperlink ref="H76" r:id="rId60" xr:uid="{3A8D2EB7-A012-4A83-86C0-51123C32DF6D}"/>
+    <hyperlink ref="H78" r:id="rId61" xr:uid="{AC284DEA-756B-4D18-AE9D-12965059EDBE}"/>
+    <hyperlink ref="H84" r:id="rId62" xr:uid="{DCB82540-1BA3-48F9-96A2-791F42A64434}"/>
+    <hyperlink ref="H85" r:id="rId63" xr:uid="{B9381049-251F-42B9-84B0-1EA59178B672}"/>
+    <hyperlink ref="H86" r:id="rId64" xr:uid="{540E3A03-74BD-4CEB-8971-9A006BEFCDF0}"/>
+    <hyperlink ref="H87" r:id="rId65" xr:uid="{72F8223A-C2F2-4F21-BABB-B8498B257A0D}"/>
+    <hyperlink ref="H88" r:id="rId66" xr:uid="{0C61D723-5ABB-4262-A872-39A6CDB6256D}"/>
+    <hyperlink ref="H89" r:id="rId67" xr:uid="{27DD1FF5-3256-41C6-B415-3EBB0EC0F4F5}"/>
+    <hyperlink ref="H93" r:id="rId68" xr:uid="{3425BE03-5207-4C7D-8D5C-A6503DADDED2}"/>
+    <hyperlink ref="H94" r:id="rId69" xr:uid="{485CFA53-D353-40F2-9341-01B79A98853E}"/>
+    <hyperlink ref="H96" r:id="rId70" xr:uid="{832E610A-F9CA-4C75-A91C-B42B0F67D4F3}"/>
+    <hyperlink ref="H97" r:id="rId71" xr:uid="{01FE6B48-CA09-4F40-B62C-9B0890D99399}"/>
+    <hyperlink ref="H3" r:id="rId72" display="https://www.lsf.tu-dortmund.de/qisserver/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=251158&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung" xr:uid="{59C03C8D-D4C1-4F3E-BE32-BECB7C56DE46}"/>
+    <hyperlink ref="H10" r:id="rId73" xr:uid="{C948447E-25EE-46B0-87D4-69726901A563}"/>
+    <hyperlink ref="H17" r:id="rId74" display="https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=vvz&amp;gguid=0xBE097E28332544129F201456DD40F8FD&amp;mode=own&amp;tguid=0x6BD942F2335C413E99E5D61BE54377E5&amp;lang=de" xr:uid="{3F957779-98BC-47BD-A023-69CBC43C874C}"/>
+    <hyperlink ref="H27" r:id="rId75" xr:uid="{58DD5441-0DE8-410C-956D-B7B8E9C3382C}"/>
+    <hyperlink ref="H64" r:id="rId76" xr:uid="{5D7A4DAF-540A-4A6F-9864-C56D22020CE4}"/>
+    <hyperlink ref="H65" r:id="rId77" xr:uid="{E793A7A2-4E6A-4865-9FD7-3E09C15CB431}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId79"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId78"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some minor fixes regarding locations on module composition
</commit_message>
<xml_diff>
--- a/KurseMscECMX_SoSe22.xlsx
+++ b/KurseMscECMX_SoSe22.xlsx
@@ -1,37 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Git_projects/ECMTX_course_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/git_projects/CourseOverview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBAB8D2-08E2-2A4E-9B08-8507BF0147D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89C8A4F-8871-DD4B-8909-40C1A8728630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="46080" windowHeight="25920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste" sheetId="8" r:id="rId1"/>
     <sheet name="Kursliste" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kursliste!$A$1:$K$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Kursliste!$A$1:$K$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Liste!$A$1:$C$38</definedName>
     <definedName name="Anfangszeit" localSheetId="0">#REF!</definedName>
     <definedName name="Anfangszeit">#REF!</definedName>
     <definedName name="Intervall" localSheetId="0">#REF!</definedName>
     <definedName name="Intervall">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="355">
   <si>
     <t>Kurs</t>
   </si>
@@ -807,9 +805,6 @@
   </si>
   <si>
     <t>https://www.oek.wiwi.uni-due.de/studium-lehre/lehrveranstaltungen/wintersemester-17-18/fortgeschrittene-oekonometrie-vorlesung-9065/</t>
-  </si>
-  <si>
-    <t>Applied Economic Policy</t>
   </si>
   <si>
     <t>Seminar Soziale Sicherung und
@@ -1052,62 +1047,68 @@
     <t>Apl. Prof. Dr. Manuel Frondel</t>
   </si>
   <si>
+    <t>https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=&amp;gguid=0x56016253C83E4BAB8F2833E781390CA2&amp;mode=&amp;tguid=0x6BD942F2335C413E99E5D61BE54377E5&amp;lang=de</t>
+  </si>
+  <si>
+    <t>Chair of Energy Economics and Applied Econometrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Empirical Macroeconomics </t>
+  </si>
+  <si>
+    <t>Apl. Prof. Dr. Torsten Schmidt</t>
+  </si>
+  <si>
+    <t>V Introduction to Empirical Macroeconomics (ruhr-uni-bochum.de)</t>
+  </si>
+  <si>
+    <t>Chair of Empirical Macroeconomics</t>
+  </si>
+  <si>
+    <t>Law and Economics</t>
+  </si>
+  <si>
+    <t>https://www.lsf.tu-dortmund.de/qisserver/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=247763&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung</t>
+  </si>
+  <si>
+    <t>Professorship of Public Economics</t>
+  </si>
+  <si>
+    <t>Prof. Galina Zudenkova, Ph.D.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Empirie der internationalen Geld- und Finanzmärkte</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Ansgar Belke</t>
+  </si>
+  <si>
+    <t>https://www.makro.wiwi.uni-due.de/studium-lehre/lehrveranstaltungen/wintersemester-21-22/empirie-der-internationalen-geld-und-finanzmaerkte-vorlesung-13695/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Energy Markets and Price Formation</t>
+  </si>
+  <si>
+    <t>https://campus.uni-due.de/lsf/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=366573&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung</t>
+  </si>
+  <si>
+    <t>Prof. Dr. Christoph Weber</t>
+  </si>
+  <si>
+    <t>Lehrstuhl für Energiewirtschaft</t>
+  </si>
+  <si>
+    <t>https://www.oek.wiwi.uni-due.de/studium-lehre/lehrveranstaltungen/sommersemester-22/fortgeschrittene-oekonometrie-vorlesung-13899/</t>
+  </si>
+  <si>
     <t xml:space="preserve">
-RWI, Essen</t>
-  </si>
-  <si>
-    <t>https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=&amp;gguid=0x56016253C83E4BAB8F2833E781390CA2&amp;mode=&amp;tguid=0x6BD942F2335C413E99E5D61BE54377E5&amp;lang=de</t>
-  </si>
-  <si>
-    <t>Chair of Energy Economics and Applied Econometrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Empirical Macroeconomics </t>
-  </si>
-  <si>
-    <t>Apl. Prof. Dr. Torsten Schmidt</t>
-  </si>
-  <si>
-    <t>V Introduction to Empirical Macroeconomics (ruhr-uni-bochum.de)</t>
-  </si>
-  <si>
-    <t>Chair of Empirical Macroeconomics</t>
-  </si>
-  <si>
-    <t>Law and Economics</t>
-  </si>
-  <si>
-    <t>https://www.lsf.tu-dortmund.de/qisserver/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=247763&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung</t>
-  </si>
-  <si>
-    <t>Professorship of Public Economics</t>
-  </si>
-  <si>
-    <t>Prof. Galina Zudenkova, Ph.D.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Empirie der internationalen Geld- und Finanzmärkte</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Ansgar Belke</t>
-  </si>
-  <si>
-    <t>https://www.makro.wiwi.uni-due.de/studium-lehre/lehrveranstaltungen/wintersemester-21-22/empirie-der-internationalen-geld-und-finanzmaerkte-vorlesung-13695/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Energy Markets and Price Formation</t>
-  </si>
-  <si>
-    <t>https://campus.uni-due.de/lsf/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=366573&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung</t>
-  </si>
-  <si>
-    <t>Prof. Dr. Christoph Weber</t>
-  </si>
-  <si>
-    <t>Lehrstuhl für Energiewirtschaft</t>
-  </si>
-  <si>
-    <t>https://www.oek.wiwi.uni-due.de/studium-lehre/lehrveranstaltungen/sommersemester-22/fortgeschrittene-oekonometrie-vorlesung-13899/</t>
+RWI, Bochum</t>
+  </si>
+  <si>
+    <t>Programming with Python</t>
+  </si>
+  <si>
+    <t>Programming Course with R</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1322,6 +1323,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1338,7 +1352,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1497,6 +1511,20 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Excel Built-in Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2077,13 +2105,13 @@
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2347,7 +2375,7 @@
         <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
@@ -2739,13 +2767,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMD97"/>
+  <dimension ref="A1:AMD99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2824,7 +2852,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I2" s="40">
         <v>3</v>
@@ -2838,10 +2866,10 @@
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" s="31" t="str">
         <f>VLOOKUP($E3,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -2860,7 +2888,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I3" s="40">
         <v>4</v>
@@ -2896,7 +2924,7 @@
         <v>42</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I4" s="41">
         <v>5</v>
@@ -2932,7 +2960,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I5" s="41">
         <v>6</v>
@@ -2946,10 +2974,10 @@
     </row>
     <row r="6" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>141</v>
@@ -2958,7 +2986,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>53</v>
@@ -2967,7 +2995,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I6" s="41">
         <v>50</v>
@@ -3003,7 +3031,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I7" s="40">
         <v>7</v>
@@ -3039,7 +3067,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I8" s="27">
         <v>17</v>
@@ -3073,7 +3101,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I9" s="27">
         <v>18</v>
@@ -3087,28 +3115,28 @@
     </row>
     <row r="10" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I10" s="27">
         <v>19</v>
@@ -3142,7 +3170,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I11" s="27">
         <v>20</v>
@@ -3178,7 +3206,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I12" s="27">
         <v>21</v>
@@ -3214,7 +3242,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I13" s="27">
         <v>22</v>
@@ -3248,7 +3276,7 @@
         <v>10</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I14" s="27">
         <v>24</v>
@@ -3284,7 +3312,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I15" s="27">
         <v>25</v>
@@ -3320,7 +3348,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I16" s="37">
         <v>26</v>
@@ -3334,19 +3362,19 @@
     </row>
     <row r="17" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D17" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>89</v>
@@ -3355,7 +3383,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I17" s="37">
         <v>27</v>
@@ -3391,7 +3419,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I18" s="37">
         <v>28</v>
@@ -3427,7 +3455,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I19" s="27">
         <v>29</v>
@@ -3463,7 +3491,7 @@
         <v>168</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I20" s="27">
         <v>30</v>
@@ -3499,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I21" s="27">
         <v>31</v>
@@ -3535,7 +3563,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I22" s="27">
         <v>32</v>
@@ -3568,10 +3596,10 @@
         <v>89</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I23" s="27">
         <v>33</v>
@@ -3607,7 +3635,7 @@
         <v>42</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I24" s="27">
         <v>34</v>
@@ -3621,7 +3649,7 @@
     </row>
     <row r="25" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="26" t="s">
-        <v>255</v>
+        <v>95</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>95</v>
@@ -3643,7 +3671,7 @@
         <v>42</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I25" s="27">
         <v>35</v>
@@ -3679,7 +3707,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="45" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I26" s="40">
         <v>36</v>
@@ -3693,19 +3721,19 @@
     </row>
     <row r="27" spans="1:11" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>342</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>344</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>53</v>
@@ -3714,7 +3742,7 @@
         <v>10</v>
       </c>
       <c r="H27" s="45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I27" s="40">
         <v>37</v>
@@ -3750,7 +3778,7 @@
         <v>10</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I28" s="40">
         <v>38</v>
@@ -3894,7 +3922,7 @@
         <v>174</v>
       </c>
       <c r="H32" s="45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I32" s="40">
         <v>40</v>
@@ -3941,65 +3969,64 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="B34" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C34" s="14" t="str">
-        <f>VLOOKUP($E34,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
-      </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10" t="s">
+      <c r="C34" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="45"/>
-      <c r="I34" s="40">
+      <c r="H34" s="50"/>
+      <c r="I34" s="51">
         <v>41</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="K34" s="10" t="s">
+      <c r="K34" s="48" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="19" t="s">
-        <v>57</v>
+        <v>353</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="C35" s="14" t="str">
         <f>VLOOKUP($E35,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Applied Economics</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="45" t="s">
-        <v>271</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H35" s="45"/>
       <c r="I35" s="40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>37</v>
@@ -4010,20 +4037,20 @@
     </row>
     <row r="36" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="19" t="s">
-        <v>243</v>
+        <v>176</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="C36" s="14" t="str">
         <f>VLOOKUP($E36,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Applied Economics</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>53</v>
@@ -4031,32 +4058,30 @@
       <c r="G36" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="45" t="s">
-        <v>311</v>
-      </c>
+      <c r="H36" s="45"/>
       <c r="I36" s="40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>37</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C37" s="14" t="str">
         <f>VLOOKUP($E37,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Professorship of Applied Economics</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>52</v>
@@ -4065,52 +4090,52 @@
         <v>53</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H37" s="45" t="s">
-        <v>312</v>
+        <v>270</v>
       </c>
       <c r="I37" s="40">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>37</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="19" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="14" t="str">
         <f>VLOOKUP($E38,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Finance</v>
+        <v>Professorship of Applied Economics</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H38" s="45" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I38" s="40">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>108</v>
@@ -4118,53 +4143,53 @@
     </row>
     <row r="39" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="19" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C39" s="14" t="str">
         <f>VLOOKUP($E39,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Professorship of Finance</v>
+        <v>Professorship of Applied Economics</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H39" s="45" t="s">
-        <v>272</v>
-      </c>
-      <c r="I39" s="42">
-        <v>45</v>
+        <v>311</v>
+      </c>
+      <c r="I39" s="40">
+        <v>43</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="19" t="s">
-        <v>274</v>
+        <v>102</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C40" s="14" t="str">
         <f>VLOOKUP($E40,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Professorship of Finance</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>60</v>
@@ -4173,13 +4198,13 @@
         <v>53</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="H40" s="45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I40" s="40">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>11</v>
@@ -4190,20 +4215,20 @@
     </row>
     <row r="41" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C41" s="14" t="str">
         <f>VLOOKUP($E41,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Economic Policy</v>
+        <v>Professorship of Finance</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>53</v>
@@ -4212,13 +4237,13 @@
         <v>10</v>
       </c>
       <c r="H41" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="I41" s="40">
-        <v>47</v>
+        <v>271</v>
+      </c>
+      <c r="I41" s="42">
+        <v>45</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K41" s="10" t="s">
         <v>109</v>
@@ -4226,18 +4251,20 @@
     </row>
     <row r="42" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="19" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>178</v>
+        <v>78</v>
       </c>
       <c r="C42" s="14" t="str">
         <f>VLOOKUP($E42,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Economic Policy</v>
-      </c>
-      <c r="D42" s="10"/>
+        <v>Professorship of Finance</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="E42" s="10" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>53</v>
@@ -4246,13 +4273,13 @@
         <v>42</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I42" s="40">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K42" s="10" t="s">
         <v>108</v>
@@ -4260,127 +4287,126 @@
     </row>
     <row r="43" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="19" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="31" t="str">
+        <v>76</v>
+      </c>
+      <c r="C43" s="14" t="str">
         <f>VLOOKUP($E43,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
-      </c>
-      <c r="D43" s="19" t="s">
+        <v>Chair of Economic Policy</v>
+      </c>
+      <c r="D43" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F43" s="19" t="s">
+      <c r="E43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="19" t="s">
-        <v>42</v>
+      <c r="G43" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H43" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="I43" s="41">
-        <v>50</v>
-      </c>
-      <c r="J43" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="I43" s="40">
+        <v>47</v>
+      </c>
+      <c r="J43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K43" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K43" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="19" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="C44" s="14" t="str">
         <f>VLOOKUP($E44,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistical Methods for Big Data</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>113</v>
+        <v>Chair of Economic Policy</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="10" t="s">
         <v>42</v>
       </c>
       <c r="H44" s="45" t="s">
-        <v>316</v>
-      </c>
-      <c r="I44" s="41">
-        <v>50</v>
-      </c>
-      <c r="J44" s="19" t="s">
-        <v>37</v>
+        <v>314</v>
+      </c>
+      <c r="I44" s="40">
+        <v>48</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="K44" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" s="20" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="19" t="s">
-        <v>266</v>
+        <v>54</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>8</v>
+        <v>110</v>
+      </c>
+      <c r="C45" s="31" t="str">
+        <f>VLOOKUP($E45,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Faculty of Statistics</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="F45" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F45" s="19" t="s">
         <v>53</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H45" s="45" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="I45" s="41">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K45" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="19" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C46" s="14" t="str">
         <f>VLOOKUP($E46,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
+        <v>Chair of Statistical Methods for Big Data</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>53</v>
@@ -4388,69 +4414,70 @@
       <c r="G46" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="45"/>
-      <c r="I46" s="40">
+      <c r="H46" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="I46" s="41">
         <v>50</v>
       </c>
       <c r="J46" s="19" t="s">
         <v>37</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="19" t="s">
-        <v>63</v>
+        <v>265</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="14" t="str">
-        <f>VLOOKUP($E47,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Mathematical Statistics with Applications in Biometrics</v>
+        <v>265</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>64</v>
+        <v>267</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H47" s="45" t="s">
-        <v>317</v>
-      </c>
-      <c r="I47" s="40">
-        <v>50</v>
+        <v>266</v>
+      </c>
+      <c r="I47" s="41">
+        <v>49</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="B48" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C48" s="14" t="str">
         <f>VLOOKUP($E48,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Business and Social Statistics</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>53</v>
@@ -4458,9 +4485,7 @@
       <c r="G48" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H48" s="45" t="s">
-        <v>276</v>
-      </c>
+      <c r="H48" s="45"/>
       <c r="I48" s="40">
         <v>50</v>
       </c>
@@ -4473,28 +4498,30 @@
     </row>
     <row r="49" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="B49" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C49" s="14" t="str">
         <f>VLOOKUP($E49,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
+        <v>Chair of Mathematical Statistics with Applications in Biometrics</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H49" s="45"/>
+        <v>16</v>
+      </c>
+      <c r="H49" s="45" t="s">
+        <v>316</v>
+      </c>
       <c r="I49" s="40">
         <v>50</v>
       </c>
@@ -4502,25 +4529,25 @@
         <v>37</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B50" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C50" s="14" t="str">
         <f>VLOOKUP($E50,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Faculty of Statistics</v>
+        <v>Chair of Business and Social Statistics</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>53</v>
@@ -4528,9 +4555,11 @@
       <c r="G50" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H50" s="45"/>
+      <c r="H50" s="45" t="s">
+        <v>275</v>
+      </c>
       <c r="I50" s="40">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J50" s="19" t="s">
         <v>37</v>
@@ -4541,9 +4570,9 @@
     </row>
     <row r="51" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="43" t="s">
         <v>110</v>
       </c>
       <c r="C51" s="14" t="str">
@@ -4551,7 +4580,7 @@
         <v>Faculty of Statistics</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>140</v>
@@ -4562,9 +4591,7 @@
       <c r="G51" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="45" t="s">
-        <v>235</v>
-      </c>
+      <c r="H51" s="45"/>
       <c r="I51" s="40">
         <v>50</v>
       </c>
@@ -4577,7 +4604,7 @@
     </row>
     <row r="52" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="19" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>110</v>
@@ -4598,11 +4625,9 @@
       <c r="G52" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H52" s="45" t="s">
-        <v>236</v>
-      </c>
+      <c r="H52" s="45"/>
       <c r="I52" s="40">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J52" s="19" t="s">
         <v>37</v>
@@ -4613,7 +4638,7 @@
     </row>
     <row r="53" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="19" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>110</v>
@@ -4635,7 +4660,7 @@
         <v>42</v>
       </c>
       <c r="H53" s="45" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I53" s="40">
         <v>50</v>
@@ -4649,17 +4674,17 @@
     </row>
     <row r="54" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="19" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="29" t="str">
+      <c r="C54" s="14" t="str">
         <f>VLOOKUP($E54,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>140</v>
@@ -4671,7 +4696,7 @@
         <v>42</v>
       </c>
       <c r="H54" s="45" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I54" s="40">
         <v>50</v>
@@ -4685,7 +4710,7 @@
     </row>
     <row r="55" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="19" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>110</v>
@@ -4707,7 +4732,7 @@
         <v>42</v>
       </c>
       <c r="H55" s="45" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I55" s="40">
         <v>50</v>
@@ -4721,17 +4746,17 @@
     </row>
     <row r="56" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="14" t="str">
+      <c r="C56" s="29" t="str">
         <f>VLOOKUP($E56,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>140</v>
@@ -4743,7 +4768,7 @@
         <v>42</v>
       </c>
       <c r="H56" s="45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I56" s="40">
         <v>50</v>
@@ -4757,7 +4782,7 @@
     </row>
     <row r="57" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="19" t="s">
-        <v>181</v>
+        <v>116</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>110</v>
@@ -4767,7 +4792,7 @@
         <v>Faculty of Statistics</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>319</v>
+        <v>14</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>140</v>
@@ -4779,7 +4804,7 @@
         <v>42</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>318</v>
+        <v>239</v>
       </c>
       <c r="I57" s="40">
         <v>50</v>
@@ -4793,7 +4818,7 @@
     </row>
     <row r="58" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>110</v>
@@ -4815,7 +4840,7 @@
         <v>42</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I58" s="40">
         <v>50</v>
@@ -4829,19 +4854,19 @@
     </row>
     <row r="59" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C59" s="14" t="str">
         <f>VLOOKUP($E59,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Faculty of Statistics</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>140</v>
       </c>
       <c r="F59" s="10" t="s">
@@ -4850,11 +4875,13 @@
       <c r="G59" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H59" s="45"/>
+      <c r="H59" s="45" t="s">
+        <v>317</v>
+      </c>
       <c r="I59" s="40">
-        <v>52</v>
-      </c>
-      <c r="J59" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>37</v>
       </c>
       <c r="K59" s="10" t="s">
@@ -4863,20 +4890,20 @@
     </row>
     <row r="60" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="19" t="s">
-        <v>265</v>
+        <v>85</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C60" s="14" t="str">
         <f>VLOOKUP($E60,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Business and Social Statistics</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>138</v>
+        <v>14</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>53</v>
@@ -4885,12 +4912,12 @@
         <v>42</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="I60" s="40">
-        <v>52</v>
-      </c>
-      <c r="J60" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J60" s="19" t="s">
         <v>37</v>
       </c>
       <c r="K60" s="10" t="s">
@@ -4899,35 +4926,33 @@
     </row>
     <row r="61" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="19" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C61" s="14" t="str">
         <f>VLOOKUP($E61,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Artificial Intelligence</v>
+        <v>Faculty of Statistics</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>183</v>
+        <v>8</v>
+      </c>
+      <c r="E61" s="44" t="s">
+        <v>140</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" s="45" t="s">
-        <v>277</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H61" s="45"/>
       <c r="I61" s="40">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K61" s="10" t="s">
         <v>109</v>
@@ -4935,248 +4960,248 @@
     </row>
     <row r="62" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="14" t="str">
+        <f>VLOOKUP($E62,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Business and Social Statistics</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H62" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="I62" s="40">
+        <v>52</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K62" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="14" t="str">
+        <f>VLOOKUP($E63,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Artificial Intelligence</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="I63" s="40">
+        <v>53</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K63" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B64" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C62" s="31" t="str">
-        <f>VLOOKUP($E62,Liste!$A$2:$C$38,2,FALSE)</f>
+      <c r="C64" s="31" t="str">
+        <f>VLOOKUP($E64,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Artificial Intelligence</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D64" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E64" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="F62" s="19" t="s">
+      <c r="F64" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G62" s="19"/>
-      <c r="H62" s="45" t="s">
+      <c r="G64" s="19"/>
+      <c r="H64" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="I62" s="41">
+      <c r="I64" s="41">
         <v>54</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="J64" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K62" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="21" t="s">
+      <c r="K64" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B65" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="15" t="str">
-        <f>VLOOKUP($E63,Liste!$A$2:$C$38,2,FALSE)</f>
+      <c r="C65" s="15" t="str">
+        <f>VLOOKUP($E65,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Environmental Economics,
  esp. Economics of Renewable Energy</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D65" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E65" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>278</v>
-      </c>
-      <c r="I63" s="39">
-        <v>55</v>
-      </c>
-      <c r="J63" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K63" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>348</v>
-      </c>
-      <c r="I64" s="39">
-        <v>56</v>
-      </c>
-      <c r="J64" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K64" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="21" t="s">
-        <v>349</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E65" s="11" t="s">
-        <v>351</v>
       </c>
       <c r="F65" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H65" s="47" t="s">
-        <v>350</v>
+        <v>10</v>
+      </c>
+      <c r="H65" s="45" t="s">
+        <v>277</v>
       </c>
       <c r="I65" s="39">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J65" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K65" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="21" t="s">
-        <v>20</v>
+        <v>344</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="15" t="str">
-        <f>VLOOKUP($E66,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Microeconomics</v>
+        <v>344</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>21</v>
+        <v>345</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>279</v>
-      </c>
-      <c r="I66" s="24">
-        <v>58</v>
-      </c>
-      <c r="J66" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K66" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="I66" s="39">
+        <v>56</v>
+      </c>
+      <c r="J66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K66" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="21" t="s">
-        <v>184</v>
+        <v>347</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C67" s="15" t="str">
-        <f>VLOOKUP($E67,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of International Economics</v>
+        <v>347</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>350</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>33</v>
+        <v>349</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G67" s="22" t="s">
+      <c r="G67" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H67" s="45" t="s">
-        <v>320</v>
-      </c>
-      <c r="I67" s="24">
-        <v>59</v>
-      </c>
-      <c r="J67" s="23" t="s">
+      <c r="H67" s="47" t="s">
+        <v>348</v>
+      </c>
+      <c r="I67" s="39">
+        <v>57</v>
+      </c>
+      <c r="J67" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K67" s="25" t="s">
+      <c r="K67" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="21" t="s">
-        <v>185</v>
+        <v>20</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>185</v>
+        <v>20</v>
       </c>
       <c r="C68" s="15" t="str">
         <f>VLOOKUP($E68,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
+        <v>Chair of Microeconomics</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G68" s="22" t="s">
         <v>10</v>
       </c>
       <c r="H68" s="45" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I68" s="24">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K68" s="25" t="s">
         <v>109</v>
@@ -5184,92 +5209,92 @@
     </row>
     <row r="69" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B69" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="35" t="str">
+        <v>184</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" s="15" t="str">
         <f>VLOOKUP($E69,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
-      </c>
-      <c r="D69" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F69" s="21" t="s">
+        <v>Chair of International Economics</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="21" t="s">
+      <c r="G69" s="22" t="s">
         <v>16</v>
       </c>
       <c r="H69" s="45" t="s">
-        <v>321</v>
-      </c>
-      <c r="I69" s="36">
-        <v>61</v>
-      </c>
-      <c r="J69" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="I69" s="24">
+        <v>59</v>
+      </c>
+      <c r="J69" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K69" s="21" t="s">
+      <c r="K69" s="25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="21" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="C70" s="15" t="str">
         <f>VLOOKUP($E70,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Microeconomics</v>
+        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="F70" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G70" s="22" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H70" s="45" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="I70" s="24">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J70" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K70" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C71" s="35" t="str">
         <f>VLOOKUP($E71,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="21" t="s">
-        <v>147</v>
+        <v>25</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="F71" s="21" t="s">
         <v>9</v>
@@ -5278,10 +5303,10 @@
         <v>16</v>
       </c>
       <c r="H71" s="45" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I71" s="36">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J71" s="21" t="s">
         <v>11</v>
@@ -5292,299 +5317,299 @@
     </row>
     <row r="72" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="B72" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" s="35" t="str">
+        <v>40</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="15" t="str">
         <f>VLOOKUP($E72,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
-      </c>
-      <c r="D72" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F72" s="21" t="s">
+        <v>Chair of Microeconomics</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G72" s="21" t="s">
-        <v>10</v>
+      <c r="G72" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="I72" s="36">
-        <v>64</v>
-      </c>
-      <c r="J72" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K72" s="21" t="s">
-        <v>109</v>
+        <v>321</v>
+      </c>
+      <c r="I72" s="24">
+        <v>62</v>
+      </c>
+      <c r="J72" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K72" s="25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="21" t="s">
-        <v>256</v>
+        <v>149</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="C73" s="15" t="str">
+        <v>149</v>
+      </c>
+      <c r="C73" s="35" t="str">
         <f>VLOOKUP($E73,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Public Economics</v>
-      </c>
-      <c r="D73" s="11" t="s">
+        <v>Chair of Labour and Health Economics</v>
+      </c>
+      <c r="D73" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F73" s="11" t="s">
+      <c r="E73" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G73" s="22" t="s">
+      <c r="G73" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H73" s="45" t="s">
-        <v>248</v>
-      </c>
-      <c r="I73" s="24">
-        <v>65</v>
-      </c>
-      <c r="J73" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K73" s="25" t="s">
-        <v>109</v>
+        <v>322</v>
+      </c>
+      <c r="I73" s="36">
+        <v>63</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K73" s="21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C74" s="15" t="str">
+        <v>186</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="35" t="str">
         <f>VLOOKUP($E74,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Finance</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F74" s="11" t="s">
+        <v>Lehrstuhl für Arbeitsmarkt- und Migrationsökonomik</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G74" s="22" t="s">
-        <v>16</v>
+      <c r="G74" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="H74" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="I74" s="24">
-        <v>67</v>
-      </c>
-      <c r="J74" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K74" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="I74" s="36">
+        <v>64</v>
+      </c>
+      <c r="J74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K74" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>106</v>
+        <v>255</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>255</v>
       </c>
       <c r="C75" s="15" t="str">
         <f>VLOOKUP($E75,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of Public Economics</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F75" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G75" s="22" t="s">
         <v>16</v>
       </c>
       <c r="H75" s="45" t="s">
-        <v>324</v>
-      </c>
-      <c r="I75" s="39">
-        <v>69</v>
-      </c>
-      <c r="J75" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K75" s="11" t="s">
-        <v>108</v>
+        <v>248</v>
+      </c>
+      <c r="I75" s="24">
+        <v>65</v>
+      </c>
+      <c r="J75" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K75" s="25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B76" s="21" t="s">
-        <v>187</v>
+        <v>47</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C76" s="15" t="str">
         <f>VLOOKUP($E76,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Chair of Finance</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>147</v>
+        <v>48</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G76" s="11" t="s">
-        <v>10</v>
+      <c r="G76" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="H76" s="45" t="s">
-        <v>282</v>
-      </c>
-      <c r="I76" s="39">
-        <v>70</v>
-      </c>
-      <c r="J76" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="I76" s="24">
+        <v>67</v>
+      </c>
+      <c r="J76" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K76" s="11" t="s">
+      <c r="K76" s="25" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="21" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="C77" s="15" t="str">
         <f>VLOOKUP($E77,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Econometrics</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="I77" s="39">
+        <v>69</v>
+      </c>
+      <c r="J77" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K77" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="15" t="str">
+        <f>VLOOKUP($E78,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Labour and Health Economics</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="I78" s="39">
+        <v>70</v>
+      </c>
+      <c r="J78" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="15" t="str">
+        <f>VLOOKUP($E79,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Environmental Economics,
  esp. Economics of Renewable Energy</v>
       </c>
-      <c r="D77" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H77" s="45" t="s">
-        <v>325</v>
-      </c>
-      <c r="I77" s="24">
-        <v>71</v>
-      </c>
-      <c r="J77" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K77" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" s="15" t="str">
-        <f>VLOOKUP($E78,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H78" s="45" t="s">
-        <v>326</v>
-      </c>
-      <c r="I78" s="24">
-        <v>72</v>
-      </c>
-      <c r="J78" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K78" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C79" s="15" t="str">
-        <f>VLOOKUP($E79,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Finance</v>
-      </c>
       <c r="D79" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>190</v>
+        <v>9</v>
       </c>
       <c r="G79" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H79" s="45" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="I79" s="24">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C80" s="15" t="str">
         <f>VLOOKUP($E80,Liste!$A$2:$C$38,2,FALSE)</f>
@@ -5600,52 +5625,52 @@
         <v>9</v>
       </c>
       <c r="G80" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H80" s="45" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="I80" s="24">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J80" s="23" t="s">
         <v>23</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="21" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="C81" s="15" t="str">
         <f>VLOOKUP($E81,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair for Energy Trading and Finance</v>
+        <v>Chair of Finance</v>
       </c>
       <c r="D81" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G81" s="22" t="s">
         <v>10</v>
       </c>
       <c r="H81" s="45" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I81" s="24">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>109</v>
@@ -5653,20 +5678,20 @@
     </row>
     <row r="82" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C82" s="15" t="str">
         <f>VLOOKUP($E82,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair for Energy Trading and Finance</v>
+        <v>Chair of Statistics</v>
       </c>
       <c r="D82" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>9</v>
@@ -5675,13 +5700,13 @@
         <v>10</v>
       </c>
       <c r="H82" s="45" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I82" s="24">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K82" s="25" t="s">
         <v>109</v>
@@ -5689,20 +5714,20 @@
     </row>
     <row r="83" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C83" s="15" t="str">
         <f>VLOOKUP($E83,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Health Economics</v>
+        <v>Chair for Energy Trading and Finance</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F83" s="11" t="s">
         <v>9</v>
@@ -5711,10 +5736,10 @@
         <v>10</v>
       </c>
       <c r="H83" s="45" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I83" s="24">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J83" s="23" t="s">
         <v>11</v>
@@ -5725,144 +5750,144 @@
     </row>
     <row r="84" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B84" s="21" t="s">
-        <v>191</v>
+        <v>31</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C84" s="15" t="str">
         <f>VLOOKUP($E84,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Labour and Health Economics</v>
+        <v>Chair for Energy Trading and Finance</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>147</v>
+        <v>30</v>
       </c>
       <c r="F84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H84" s="45" t="s">
-        <v>327</v>
+        <v>285</v>
       </c>
       <c r="I84" s="24">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J84" s="23" t="s">
         <v>11</v>
       </c>
       <c r="K84" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C85" s="15" t="str">
         <f>VLOOKUP($E85,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Health Economics</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="45" t="s">
+        <v>286</v>
+      </c>
+      <c r="I85" s="24">
+        <v>78</v>
+      </c>
+      <c r="J85" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K85" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="15" t="str">
+        <f>VLOOKUP($E86,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Labour and Health Economics</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="I86" s="24">
+        <v>79</v>
+      </c>
+      <c r="J86" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K86" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="15" t="str">
+        <f>VLOOKUP($E87,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Environmental Economics,
  esp. Economics of Renewable Energy</v>
       </c>
-      <c r="D85" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H85" s="45" t="s">
-        <v>247</v>
-      </c>
-      <c r="I85" s="24">
-        <v>81</v>
-      </c>
-      <c r="J85" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K85" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C86" s="15" t="str">
-        <f>VLOOKUP($E86,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F86" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H86" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="I86" s="24">
-        <v>82</v>
-      </c>
-      <c r="J86" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K86" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C87" s="15" t="str">
-        <f>VLOOKUP($E87,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of International Economics</v>
-      </c>
       <c r="D87" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G87" s="22" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H87" s="45" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I87" s="24">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>109</v>
@@ -5870,71 +5895,71 @@
     </row>
     <row r="88" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="21" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="C88" s="15" t="str">
         <f>VLOOKUP($E88,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair for Energy Trading and Finance</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F88" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G88" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H88" s="45" t="s">
-        <v>328</v>
+        <v>250</v>
       </c>
       <c r="I88" s="24">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J88" s="23" t="s">
         <v>11</v>
       </c>
       <c r="K88" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="21" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C89" s="15" t="str">
         <f>VLOOKUP($E89,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of International Economics</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F89" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="H89" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I89" s="24">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J89" s="23" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="K89" s="25" t="s">
         <v>109</v>
@@ -5942,43 +5967,43 @@
     </row>
     <row r="90" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C90" s="15" t="str">
         <f>VLOOKUP($E90,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair for Energy Trading and Finance</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F90" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G90" s="22" t="s">
-        <v>168</v>
+        <v>16</v>
       </c>
       <c r="H90" s="45" t="s">
-        <v>253</v>
+        <v>327</v>
       </c>
       <c r="I90" s="24">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J90" s="23" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="K90" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="21" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>13</v>
@@ -6000,7 +6025,7 @@
         <v>168</v>
       </c>
       <c r="H91" s="45" t="s">
-        <v>353</v>
+        <v>252</v>
       </c>
       <c r="I91" s="24">
         <v>86</v>
@@ -6009,12 +6034,12 @@
         <v>37</v>
       </c>
       <c r="K91" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="21" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>13</v>
@@ -6036,7 +6061,7 @@
         <v>168</v>
       </c>
       <c r="H92" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I92" s="24">
         <v>86</v>
@@ -6050,35 +6075,35 @@
     </row>
     <row r="93" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="21" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C93" s="15" t="str">
         <f>VLOOKUP($E93,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Health Economics</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F93" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G93" s="22" t="s">
-        <v>16</v>
+        <v>168</v>
       </c>
       <c r="H93" s="45" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="I93" s="24">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J93" s="23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="K93" s="25" t="s">
         <v>108</v>
@@ -6086,17 +6111,17 @@
     </row>
     <row r="94" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="21" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>192</v>
+        <v>13</v>
       </c>
       <c r="C94" s="15" t="str">
         <f>VLOOKUP($E94,Liste!$A$2:$C$38,2,FALSE)</f>
         <v>Chair of Econometrics</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>15</v>
@@ -6105,13 +6130,13 @@
         <v>9</v>
       </c>
       <c r="G94" s="22" t="s">
-        <v>10</v>
+        <v>168</v>
       </c>
       <c r="H94" s="45" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="I94" s="24">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J94" s="23" t="s">
         <v>37</v>
@@ -6122,20 +6147,20 @@
     </row>
     <row r="95" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="21" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C95" s="15" t="str">
         <f>VLOOKUP($E95,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
+        <v>Chair of Health Economics</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F95" s="11" t="s">
         <v>9</v>
@@ -6144,94 +6169,166 @@
         <v>16</v>
       </c>
       <c r="H95" s="45" t="s">
-        <v>231</v>
+        <v>328</v>
       </c>
       <c r="I95" s="24">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J95" s="23" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="K95" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
       <c r="C96" s="15" t="str">
         <f>VLOOKUP($E96,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Statistics</v>
+        <v>Chair of Econometrics</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F96" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G96" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>330</v>
+        <v>290</v>
       </c>
       <c r="I96" s="24">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J96" s="23" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K96" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="21" t="s">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>289</v>
+        <v>43</v>
       </c>
       <c r="C97" s="15" t="str">
         <f>VLOOKUP($E97,Liste!$A$2:$C$38,2,FALSE)</f>
-        <v>Chair of Econometrics</v>
+        <v>Chair of Statistics</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F97" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G97" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H97" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="I97" s="24">
+        <v>91</v>
+      </c>
+      <c r="J97" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K97" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" s="15" t="str">
+        <f>VLOOKUP($E98,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Statistics</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="I98" s="24">
+        <v>93</v>
+      </c>
+      <c r="J98" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K98" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C99" s="15" t="str">
+        <f>VLOOKUP($E99,Liste!$A$2:$C$38,2,FALSE)</f>
+        <v>Chair of Econometrics</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H97" s="45" t="s">
-        <v>290</v>
-      </c>
-      <c r="I97" s="24">
+      <c r="H99" s="45" t="s">
+        <v>289</v>
+      </c>
+      <c r="I99" s="24">
         <v>5</v>
       </c>
-      <c r="J97" s="23" t="s">
+      <c r="J99" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K97" s="25" t="s">
+      <c r="K99" s="25" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="U54" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a day from the list. Select CANCEL, and then press ALT+DOWN ARROW to select from the drop-down list" sqref="U56" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"SONNTAG,MONTAG,DIENSTAG,MITTWOCH,DONNERSTAG,FREITAG,SAMSTAG"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6247,24 +6344,24 @@
     <hyperlink ref="H31" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
     <hyperlink ref="H32" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
     <hyperlink ref="H33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="H37" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="H38" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="H39" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="H40" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="H77" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="H90" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="H95" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="H39" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="H40" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="H41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="H42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="H79" r:id="rId15" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="H92" r:id="rId16" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="H97" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
     <hyperlink ref="H2" r:id="rId18" xr:uid="{2B7F445A-4010-5D45-8B72-1E7FF5B85AC2}"/>
-    <hyperlink ref="H35" r:id="rId19" xr:uid="{60BFBEE5-076F-A64C-A225-ADEE1C4BD7CB}"/>
-    <hyperlink ref="H42" r:id="rId20" xr:uid="{23808E95-1E7A-0746-B8FD-00EDF2C86A74}"/>
-    <hyperlink ref="H61" r:id="rId21" xr:uid="{C2A1EBF8-E857-D545-B0EF-49D7097B7749}"/>
-    <hyperlink ref="H63" r:id="rId22" xr:uid="{7E63E588-49BB-D143-B9B4-E7580E586BAA}"/>
-    <hyperlink ref="H66" r:id="rId23" xr:uid="{F9FB12F0-5F1E-4143-8431-A414F19C6FF0}"/>
-    <hyperlink ref="H70" r:id="rId24" xr:uid="{9ADB501C-CF4E-DE42-829E-1B0FF8166250}"/>
-    <hyperlink ref="H79" r:id="rId25" xr:uid="{732233EA-CE2C-9B48-A34F-19AD7FDC6D2C}"/>
-    <hyperlink ref="H80" r:id="rId26" xr:uid="{4DCAD565-04BA-AD49-AD0C-4AFEB7188DCC}"/>
-    <hyperlink ref="H81" r:id="rId27" xr:uid="{F5282177-DF5F-F44C-963E-976E7C656D83}"/>
-    <hyperlink ref="H83" r:id="rId28" xr:uid="{71243A51-6FC6-E34C-90BE-9947021EA4E1}"/>
+    <hyperlink ref="H37" r:id="rId19" xr:uid="{60BFBEE5-076F-A64C-A225-ADEE1C4BD7CB}"/>
+    <hyperlink ref="H44" r:id="rId20" xr:uid="{23808E95-1E7A-0746-B8FD-00EDF2C86A74}"/>
+    <hyperlink ref="H63" r:id="rId21" xr:uid="{C2A1EBF8-E857-D545-B0EF-49D7097B7749}"/>
+    <hyperlink ref="H65" r:id="rId22" xr:uid="{7E63E588-49BB-D143-B9B4-E7580E586BAA}"/>
+    <hyperlink ref="H68" r:id="rId23" xr:uid="{F9FB12F0-5F1E-4143-8431-A414F19C6FF0}"/>
+    <hyperlink ref="H72" r:id="rId24" xr:uid="{9ADB501C-CF4E-DE42-829E-1B0FF8166250}"/>
+    <hyperlink ref="H81" r:id="rId25" xr:uid="{732233EA-CE2C-9B48-A34F-19AD7FDC6D2C}"/>
+    <hyperlink ref="H82" r:id="rId26" xr:uid="{4DCAD565-04BA-AD49-AD0C-4AFEB7188DCC}"/>
+    <hyperlink ref="H83" r:id="rId27" xr:uid="{F5282177-DF5F-F44C-963E-976E7C656D83}"/>
+    <hyperlink ref="H85" r:id="rId28" xr:uid="{71243A51-6FC6-E34C-90BE-9947021EA4E1}"/>
     <hyperlink ref="H11" r:id="rId29" xr:uid="{DF1DAC8E-3F75-5846-952C-CFDFFAADB7CF}"/>
     <hyperlink ref="H9" r:id="rId30" xr:uid="{8FB1C5CC-891B-4E45-819E-AEE1319C1CC3}"/>
     <hyperlink ref="H13" r:id="rId31" xr:uid="{9BAEA748-035C-C844-AFBA-2E88BB1B1519}"/>
@@ -6281,39 +6378,39 @@
     <hyperlink ref="H24" r:id="rId42" xr:uid="{F3180EAA-200E-4AC7-A0C2-68DA341AE008}"/>
     <hyperlink ref="H25" r:id="rId43" xr:uid="{9EEC934C-FC80-420E-B966-1EF8E82DD430}"/>
     <hyperlink ref="H30" r:id="rId44" location="basicdata" xr:uid="{8C0E0B15-F2D7-4152-8A3A-C4B63DC2342A}"/>
-    <hyperlink ref="H36" r:id="rId45" xr:uid="{4DD54FB2-9139-48B1-BBCF-5D5471DAECD0}"/>
-    <hyperlink ref="H43" r:id="rId46" xr:uid="{E0310F6A-80BB-4666-B128-ABFA174004B5}"/>
-    <hyperlink ref="H44" r:id="rId47" xr:uid="{A49BCD15-895A-47E3-B38F-119C48F96EC2}"/>
-    <hyperlink ref="H47" r:id="rId48" xr:uid="{912D2986-EA6B-4EF8-8161-EB8B9777A1EA}"/>
-    <hyperlink ref="H57" r:id="rId49" xr:uid="{E4EC41F5-9B9D-4A2E-9C8D-085442A52492}"/>
-    <hyperlink ref="H58" r:id="rId50" xr:uid="{16CE3935-D21A-4C5B-82EA-1CDF0C5792B4}"/>
-    <hyperlink ref="H60" r:id="rId51" xr:uid="{95987F1E-714E-475F-9F37-BFF46E5FF853}"/>
-    <hyperlink ref="H62" r:id="rId52" xr:uid="{5573F406-C721-42E7-B33B-F5125403275C}"/>
-    <hyperlink ref="H67" r:id="rId53" xr:uid="{B09486E6-3BCF-4C35-89F1-0F55C6E5C422}"/>
-    <hyperlink ref="H69" r:id="rId54" xr:uid="{D7159F27-BE69-4A6A-88E6-12AA0DFC22B1}"/>
-    <hyperlink ref="H71" r:id="rId55" xr:uid="{32F7EAFF-4E97-4C42-B31A-A0EEEAB574D8}"/>
-    <hyperlink ref="H72" r:id="rId56" xr:uid="{BBE37BEB-91BB-454E-8C75-B096251E564C}"/>
-    <hyperlink ref="H73" r:id="rId57" xr:uid="{4246FEB6-B0C6-4315-92FF-E09E8578C666}"/>
-    <hyperlink ref="H74" r:id="rId58" xr:uid="{C3486942-4849-4ADF-9729-57579A743CBE}"/>
-    <hyperlink ref="H75" r:id="rId59" xr:uid="{74C74B68-0088-4D8D-B81A-5280BA2E3496}"/>
-    <hyperlink ref="H76" r:id="rId60" xr:uid="{3A8D2EB7-A012-4A83-86C0-51123C32DF6D}"/>
-    <hyperlink ref="H78" r:id="rId61" xr:uid="{AC284DEA-756B-4D18-AE9D-12965059EDBE}"/>
-    <hyperlink ref="H84" r:id="rId62" xr:uid="{DCB82540-1BA3-48F9-96A2-791F42A64434}"/>
-    <hyperlink ref="H85" r:id="rId63" xr:uid="{B9381049-251F-42B9-84B0-1EA59178B672}"/>
-    <hyperlink ref="H86" r:id="rId64" xr:uid="{540E3A03-74BD-4CEB-8971-9A006BEFCDF0}"/>
-    <hyperlink ref="H87" r:id="rId65" xr:uid="{72F8223A-C2F2-4F21-BABB-B8498B257A0D}"/>
-    <hyperlink ref="H88" r:id="rId66" xr:uid="{0C61D723-5ABB-4262-A872-39A6CDB6256D}"/>
-    <hyperlink ref="H89" r:id="rId67" xr:uid="{27DD1FF5-3256-41C6-B415-3EBB0EC0F4F5}"/>
-    <hyperlink ref="H93" r:id="rId68" xr:uid="{3425BE03-5207-4C7D-8D5C-A6503DADDED2}"/>
-    <hyperlink ref="H94" r:id="rId69" xr:uid="{485CFA53-D353-40F2-9341-01B79A98853E}"/>
-    <hyperlink ref="H96" r:id="rId70" xr:uid="{832E610A-F9CA-4C75-A91C-B42B0F67D4F3}"/>
-    <hyperlink ref="H97" r:id="rId71" xr:uid="{01FE6B48-CA09-4F40-B62C-9B0890D99399}"/>
+    <hyperlink ref="H38" r:id="rId45" xr:uid="{4DD54FB2-9139-48B1-BBCF-5D5471DAECD0}"/>
+    <hyperlink ref="H45" r:id="rId46" xr:uid="{E0310F6A-80BB-4666-B128-ABFA174004B5}"/>
+    <hyperlink ref="H46" r:id="rId47" xr:uid="{A49BCD15-895A-47E3-B38F-119C48F96EC2}"/>
+    <hyperlink ref="H49" r:id="rId48" xr:uid="{912D2986-EA6B-4EF8-8161-EB8B9777A1EA}"/>
+    <hyperlink ref="H59" r:id="rId49" xr:uid="{E4EC41F5-9B9D-4A2E-9C8D-085442A52492}"/>
+    <hyperlink ref="H60" r:id="rId50" xr:uid="{16CE3935-D21A-4C5B-82EA-1CDF0C5792B4}"/>
+    <hyperlink ref="H62" r:id="rId51" xr:uid="{95987F1E-714E-475F-9F37-BFF46E5FF853}"/>
+    <hyperlink ref="H64" r:id="rId52" xr:uid="{5573F406-C721-42E7-B33B-F5125403275C}"/>
+    <hyperlink ref="H69" r:id="rId53" xr:uid="{B09486E6-3BCF-4C35-89F1-0F55C6E5C422}"/>
+    <hyperlink ref="H71" r:id="rId54" xr:uid="{D7159F27-BE69-4A6A-88E6-12AA0DFC22B1}"/>
+    <hyperlink ref="H73" r:id="rId55" xr:uid="{32F7EAFF-4E97-4C42-B31A-A0EEEAB574D8}"/>
+    <hyperlink ref="H74" r:id="rId56" xr:uid="{BBE37BEB-91BB-454E-8C75-B096251E564C}"/>
+    <hyperlink ref="H75" r:id="rId57" xr:uid="{4246FEB6-B0C6-4315-92FF-E09E8578C666}"/>
+    <hyperlink ref="H76" r:id="rId58" xr:uid="{C3486942-4849-4ADF-9729-57579A743CBE}"/>
+    <hyperlink ref="H77" r:id="rId59" xr:uid="{74C74B68-0088-4D8D-B81A-5280BA2E3496}"/>
+    <hyperlink ref="H78" r:id="rId60" xr:uid="{3A8D2EB7-A012-4A83-86C0-51123C32DF6D}"/>
+    <hyperlink ref="H80" r:id="rId61" xr:uid="{AC284DEA-756B-4D18-AE9D-12965059EDBE}"/>
+    <hyperlink ref="H86" r:id="rId62" xr:uid="{DCB82540-1BA3-48F9-96A2-791F42A64434}"/>
+    <hyperlink ref="H87" r:id="rId63" xr:uid="{B9381049-251F-42B9-84B0-1EA59178B672}"/>
+    <hyperlink ref="H88" r:id="rId64" xr:uid="{540E3A03-74BD-4CEB-8971-9A006BEFCDF0}"/>
+    <hyperlink ref="H89" r:id="rId65" xr:uid="{72F8223A-C2F2-4F21-BABB-B8498B257A0D}"/>
+    <hyperlink ref="H90" r:id="rId66" xr:uid="{0C61D723-5ABB-4262-A872-39A6CDB6256D}"/>
+    <hyperlink ref="H91" r:id="rId67" xr:uid="{27DD1FF5-3256-41C6-B415-3EBB0EC0F4F5}"/>
+    <hyperlink ref="H95" r:id="rId68" xr:uid="{3425BE03-5207-4C7D-8D5C-A6503DADDED2}"/>
+    <hyperlink ref="H96" r:id="rId69" xr:uid="{485CFA53-D353-40F2-9341-01B79A98853E}"/>
+    <hyperlink ref="H98" r:id="rId70" xr:uid="{832E610A-F9CA-4C75-A91C-B42B0F67D4F3}"/>
+    <hyperlink ref="H99" r:id="rId71" xr:uid="{01FE6B48-CA09-4F40-B62C-9B0890D99399}"/>
     <hyperlink ref="H3" r:id="rId72" display="https://www.lsf.tu-dortmund.de/qisserver/rds?state=verpublish&amp;status=init&amp;vmfile=no&amp;publishid=251158&amp;moduleCall=webInfo&amp;publishConfFile=webInfo&amp;publishSubDir=veranstaltung" xr:uid="{59C03C8D-D4C1-4F3E-BE32-BECB7C56DE46}"/>
     <hyperlink ref="H10" r:id="rId73" xr:uid="{C948447E-25EE-46B0-87D4-69726901A563}"/>
     <hyperlink ref="H17" r:id="rId74" display="https://vvz.ruhr-uni-bochum.de/campus/all/event.asp?objgguid=NEW&amp;from=vvz&amp;gguid=0xBE097E28332544129F201456DD40F8FD&amp;mode=own&amp;tguid=0x6BD942F2335C413E99E5D61BE54377E5&amp;lang=de" xr:uid="{3F957779-98BC-47BD-A023-69CBC43C874C}"/>
     <hyperlink ref="H27" r:id="rId75" xr:uid="{58DD5441-0DE8-410C-956D-B7B8E9C3382C}"/>
-    <hyperlink ref="H64" r:id="rId76" xr:uid="{5D7A4DAF-540A-4A6F-9864-C56D22020CE4}"/>
-    <hyperlink ref="H65" r:id="rId77" xr:uid="{E793A7A2-4E6A-4865-9FD7-3E09C15CB431}"/>
+    <hyperlink ref="H66" r:id="rId76" xr:uid="{5D7A4DAF-540A-4A6F-9864-C56D22020CE4}"/>
+    <hyperlink ref="H67" r:id="rId77" xr:uid="{E793A7A2-4E6A-4865-9FD7-3E09C15CB431}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId78"/>

</xml_diff>